<commit_message>
Add bit mask description
</commit_message>
<xml_diff>
--- a/Documentation/Описание битовых масок Норби2 СЭС v0.0.xlsx
+++ b/Documentation/Описание битовых масок Норби2 СЭС v0.0.xlsx
@@ -11,12 +11,12 @@
     <sheet name="Лист2" sheetId="2" r:id="rId2"/>
     <sheet name="Лист3" sheetId="3" r:id="rId3"/>
   </sheets>
-  <calcPr calcId="144525"/>
+  <calcPr calcId="145621"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="419" uniqueCount="304">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="690" uniqueCount="391">
   <si>
     <t>Состояние</t>
   </si>
@@ -33,6 +33,51 @@
     <t>Номер бит</t>
   </si>
   <si>
+    <t>PMM Error_PWR_Ch_State_CANmain</t>
+  </si>
+  <si>
+    <t>PMM Error_PWR_Ch_State_CANbackup</t>
+  </si>
+  <si>
+    <t>PMM Error_PWR_Ch_State_Vbat1_eF1</t>
+  </si>
+  <si>
+    <t>PMM Error_PWR_Ch_State_Vbat1_eF2</t>
+  </si>
+  <si>
+    <t>PMM Error_PWR_Ch_State_Vbat2_eF1</t>
+  </si>
+  <si>
+    <t>PMM Error_PWR_Ch_State_Vbat2_eF2</t>
+  </si>
+  <si>
+    <t>PMM Error_PWR_Ch_State_PBMs_Logic</t>
+  </si>
+  <si>
+    <t>PMM Error_I2C_GPIO_Ext1</t>
+  </si>
+  <si>
+    <t>PDM Error_I2C_GPIO_Ext1</t>
+  </si>
+  <si>
+    <t>PDM Error_I2C_GPIO_Ext2</t>
+  </si>
+  <si>
+    <t>PDM Error_I2C_MUX</t>
+  </si>
+  <si>
+    <t>PAM Error_State_DC_DC</t>
+  </si>
+  <si>
+    <t>PAM Error_I2C_GPIO_Ext</t>
+  </si>
+  <si>
+    <t>PAM Error_I2C_MUX_1</t>
+  </si>
+  <si>
+    <t>PAM Error_I2C_MUX_2</t>
+  </si>
+  <si>
     <t xml:space="preserve"> </t>
   </si>
   <si>
@@ -928,13 +973,229 @@
   </si>
   <si>
     <t>PBM 4 Branch 2 Auto_Corr_Capacity_Cmd</t>
+  </si>
+  <si>
+    <t>Статус Отказов (ошибок) PBM1</t>
+  </si>
+  <si>
+    <t>Error_PCA9534</t>
+  </si>
+  <si>
+    <t>Low_Energy_Flag</t>
+  </si>
+  <si>
+    <t>Zero_Energy_Flag</t>
+  </si>
+  <si>
+    <t>Heat 1 Error_INA238</t>
+  </si>
+  <si>
+    <t>Heat 1 Error_Heat</t>
+  </si>
+  <si>
+    <t>Heat 1 Error_Heat_TMP1075 1</t>
+  </si>
+  <si>
+    <t>Heat 1 Error_Heat_TMP1075 2</t>
+  </si>
+  <si>
+    <t>Heat 2 Error_INA238</t>
+  </si>
+  <si>
+    <t>Heat 2 Error_Heat</t>
+  </si>
+  <si>
+    <t>Heat 2 Error_Heat_TMP1075 1</t>
+  </si>
+  <si>
+    <t>Heat 2 Error_Heat_TMP1075 2</t>
+  </si>
+  <si>
+    <t>Branch 1 Error_Emerg_Chrg</t>
+  </si>
+  <si>
+    <t>Branch 2 Error_Emerg_Chrg</t>
+  </si>
+  <si>
+    <t xml:space="preserve">0 - OK,        1 -Error </t>
+  </si>
+  <si>
+    <t>Статус Отказов (ошибок) PBM2</t>
+  </si>
+  <si>
+    <t>Статус Отказов (ошибок) PBM3</t>
+  </si>
+  <si>
+    <t>Статус Отказов (ошибок) PBM4</t>
+  </si>
+  <si>
+    <t>Статус Отказов (ошибок) контроллер 1 PBM1</t>
+  </si>
+  <si>
+    <t>OVP</t>
+  </si>
+  <si>
+    <t xml:space="preserve">UVP </t>
+  </si>
+  <si>
+    <t>OCCP</t>
+  </si>
+  <si>
+    <t>ODCP</t>
+  </si>
+  <si>
+    <t>PreqF</t>
+  </si>
+  <si>
+    <t>Ldet</t>
+  </si>
+  <si>
+    <t>OC</t>
+  </si>
+  <si>
+    <t>OD</t>
+  </si>
+  <si>
+    <t>SC</t>
+  </si>
+  <si>
+    <t>PreqChrg</t>
+  </si>
+  <si>
+    <t>DchgControlFlag</t>
+  </si>
+  <si>
+    <t>ChgControlFlag</t>
+  </si>
+  <si>
+    <t>Error_Discharge</t>
+  </si>
+  <si>
+    <t>Error_Charge</t>
+  </si>
+  <si>
+    <t>Error_MAX17320</t>
+  </si>
+  <si>
+    <t>Статус Отказов (ошибок) контроллер 2 PBM1</t>
+  </si>
+  <si>
+    <t>Статус Отказов (ошибок) контроллер 1 PBM2</t>
+  </si>
+  <si>
+    <t>Статус Отказов (ошибок) контроллер 1 PBM3</t>
+  </si>
+  <si>
+    <t>Статус Отказов (ошибок) контроллер 2 PBM2</t>
+  </si>
+  <si>
+    <t>Статус Отказов (ошибок) контроллер 2 PBM3</t>
+  </si>
+  <si>
+    <t>Статус Отказов (ошибок) контроллер 1 PBM4</t>
+  </si>
+  <si>
+    <t>Статус Отказов (ошибок) контроллер 2 PBM4</t>
+  </si>
+  <si>
+    <t>МАЯК</t>
+  </si>
+  <si>
+    <t>Статусы отказов (ошибок)АБ, битовая маска (МАЯК), 0</t>
+  </si>
+  <si>
+    <t>Статусы отказов (ошибок)АБ, битовая маска (МАЯК), 1</t>
+  </si>
+  <si>
+    <t>Статусы отказов (ошибок)АБ, битовая маска (МАЯК), 3</t>
+  </si>
+  <si>
+    <t>PBM1 Branch1 Error_Discharge</t>
+  </si>
+  <si>
+    <t>PBM1 Branch1 Error_Charge</t>
+  </si>
+  <si>
+    <t>PBM1 Branch1 Error_MAX17320</t>
+  </si>
+  <si>
+    <t>PBM1 Branch2 Error_Discharge</t>
+  </si>
+  <si>
+    <t>PBM1 Branch2 Error_Charge</t>
+  </si>
+  <si>
+    <t>PBM1 Branch2 Error_MAX17320</t>
+  </si>
+  <si>
+    <t>PBM2 Branch1 Error_Discharge</t>
+  </si>
+  <si>
+    <t>PBM2 Branch1 Error_Charge</t>
+  </si>
+  <si>
+    <t>PBM2 Branch1 Error_MAX17320</t>
+  </si>
+  <si>
+    <t>PBM2 Branch2 Error_Discharge</t>
+  </si>
+  <si>
+    <t>PBM2 Branch2 Error_Charge</t>
+  </si>
+  <si>
+    <t>PBM2 Branch2 Error_MAX17320</t>
+  </si>
+  <si>
+    <t>PBM3 Branch1 Error_Charge</t>
+  </si>
+  <si>
+    <t>PBM3 Branch1 Error_Discharge</t>
+  </si>
+  <si>
+    <t>PBM3 Branch1 Error_MAX17320</t>
+  </si>
+  <si>
+    <t>PBM3 Branch2 Error_Discharge</t>
+  </si>
+  <si>
+    <t>PBM3 Branch2 Error_Charge</t>
+  </si>
+  <si>
+    <t>PBM3 Branch2 Error_MAX17320</t>
+  </si>
+  <si>
+    <t>PBM4 Branch1 Error_Discharge</t>
+  </si>
+  <si>
+    <t>PBM4 Branch1 Error_Charge</t>
+  </si>
+  <si>
+    <t>PBM4 Branch2 Error_MAX17320</t>
+  </si>
+  <si>
+    <t>PBM4 Branch1 Error_MAX17320</t>
+  </si>
+  <si>
+    <t>PBM4 Branch2 Error_Discharge</t>
+  </si>
+  <si>
+    <t>PBM4 Branch2 Error_Charge</t>
+  </si>
+  <si>
+    <t>Статус отказов элементов СЭС, битовая маска (МАЯК), 0</t>
+  </si>
+  <si>
+    <t>Статус отказов элементов СЭС, битовая маска (МАЯК), 1</t>
+  </si>
+  <si>
+    <t>PAM  Error_State_LDO</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -958,6 +1219,13 @@
       <charset val="204"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="36"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -967,7 +1235,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="34">
+  <borders count="35">
     <border>
       <left/>
       <right/>
@@ -1342,6 +1610,17 @@
       <right style="medium">
         <color indexed="64"/>
       </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
       <top style="medium">
         <color indexed="64"/>
       </top>
@@ -1393,7 +1672,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="56">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="10" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1437,7 +1716,6 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1477,6 +1755,9 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1557,6 +1838,19 @@
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="33" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="34" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="33" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="24" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="25" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1860,10 +2154,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B5:U150"/>
+  <dimension ref="A5:U147"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A38" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="N52" sqref="N52"/>
+    <sheetView tabSelected="1" topLeftCell="A52" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="O62" sqref="O62"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1978,7 +2272,7 @@
     </row>
     <row r="8" spans="2:21" ht="67.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B8" s="6" t="s">
-        <v>6</v>
+        <v>21</v>
       </c>
       <c r="C8" s="1">
         <v>16</v>
@@ -1987,252 +2281,252 @@
         <v>165</v>
       </c>
       <c r="E8" s="7" t="s">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="F8" s="1" t="s">
-        <v>19</v>
+        <v>34</v>
       </c>
       <c r="G8" s="2" t="s">
-        <v>19</v>
+        <v>34</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>19</v>
-      </c>
-      <c r="I8" s="19" t="s">
-        <v>19</v>
+        <v>34</v>
+      </c>
+      <c r="I8" s="18" t="s">
+        <v>34</v>
       </c>
       <c r="J8" s="8" t="s">
-        <v>18</v>
+        <v>33</v>
       </c>
       <c r="K8" s="9" t="s">
-        <v>17</v>
+        <v>32</v>
       </c>
       <c r="L8" s="9" t="s">
-        <v>16</v>
+        <v>31</v>
       </c>
       <c r="M8" s="10" t="s">
-        <v>16</v>
+        <v>31</v>
       </c>
       <c r="N8" s="12" t="s">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="O8" s="12" t="s">
-        <v>14</v>
+        <v>29</v>
       </c>
       <c r="P8" s="12" t="s">
-        <v>13</v>
-      </c>
-      <c r="Q8" s="22" t="s">
-        <v>12</v>
+        <v>28</v>
+      </c>
+      <c r="Q8" s="21" t="s">
+        <v>27</v>
       </c>
       <c r="R8" s="12" t="s">
-        <v>11</v>
+        <v>26</v>
       </c>
       <c r="S8" s="9" t="s">
-        <v>10</v>
+        <v>25</v>
       </c>
       <c r="T8" s="9" t="s">
-        <v>9</v>
+        <v>24</v>
       </c>
       <c r="U8" s="14" t="s">
-        <v>8</v>
+        <v>23</v>
       </c>
     </row>
     <row r="9" spans="2:21" ht="67.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B9" s="6" t="s">
-        <v>21</v>
-      </c>
-      <c r="C9" s="18">
+        <v>36</v>
+      </c>
+      <c r="C9" s="17">
         <v>16</v>
       </c>
-      <c r="D9" s="19">
+      <c r="D9" s="18">
         <v>167</v>
       </c>
       <c r="E9" s="7" t="s">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="F9" s="8" t="s">
-        <v>19</v>
+        <v>34</v>
       </c>
       <c r="G9" s="9" t="s">
-        <v>19</v>
+        <v>34</v>
       </c>
       <c r="H9" s="9" t="s">
-        <v>19</v>
-      </c>
-      <c r="I9" s="22" t="s">
-        <v>34</v>
+        <v>34</v>
+      </c>
+      <c r="I9" s="21" t="s">
+        <v>49</v>
       </c>
       <c r="J9" s="12" t="s">
-        <v>33</v>
+        <v>48</v>
       </c>
       <c r="K9" s="9" t="s">
-        <v>32</v>
+        <v>47</v>
       </c>
       <c r="L9" s="9" t="s">
-        <v>31</v>
+        <v>46</v>
       </c>
       <c r="M9" s="10" t="s">
-        <v>30</v>
+        <v>45</v>
       </c>
       <c r="N9" s="12" t="s">
-        <v>29</v>
+        <v>44</v>
       </c>
       <c r="O9" s="12" t="s">
-        <v>28</v>
+        <v>43</v>
       </c>
       <c r="P9" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="Q9" s="22" t="s">
-        <v>26</v>
+        <v>42</v>
+      </c>
+      <c r="Q9" s="21" t="s">
+        <v>41</v>
       </c>
       <c r="R9" s="12" t="s">
-        <v>25</v>
+        <v>40</v>
       </c>
       <c r="S9" s="9" t="s">
-        <v>24</v>
+        <v>39</v>
       </c>
       <c r="T9" s="9" t="s">
-        <v>23</v>
+        <v>38</v>
       </c>
       <c r="U9" s="14" t="s">
-        <v>22</v>
+        <v>37</v>
       </c>
     </row>
     <row r="10" spans="2:21" ht="67.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B10" s="6" t="s">
+        <v>50</v>
+      </c>
+      <c r="C10" s="17">
+        <v>16</v>
+      </c>
+      <c r="D10" s="18">
+        <v>169</v>
+      </c>
+      <c r="E10" s="7" t="s">
         <v>35</v>
       </c>
-      <c r="C10" s="18">
-        <v>16</v>
-      </c>
-      <c r="D10" s="19">
-        <v>169</v>
-      </c>
-      <c r="E10" s="7" t="s">
-        <v>20</v>
-      </c>
       <c r="F10" s="8" t="s">
+        <v>66</v>
+      </c>
+      <c r="G10" s="9" t="s">
+        <v>65</v>
+      </c>
+      <c r="H10" s="9" t="s">
+        <v>64</v>
+      </c>
+      <c r="I10" s="21" t="s">
+        <v>63</v>
+      </c>
+      <c r="J10" s="12" t="s">
+        <v>62</v>
+      </c>
+      <c r="K10" s="9" t="s">
+        <v>61</v>
+      </c>
+      <c r="L10" s="9" t="s">
+        <v>60</v>
+      </c>
+      <c r="M10" s="10" t="s">
+        <v>59</v>
+      </c>
+      <c r="N10" s="12" t="s">
+        <v>58</v>
+      </c>
+      <c r="O10" s="12" t="s">
+        <v>57</v>
+      </c>
+      <c r="P10" s="12" t="s">
+        <v>56</v>
+      </c>
+      <c r="Q10" s="21" t="s">
+        <v>55</v>
+      </c>
+      <c r="R10" s="12" t="s">
+        <v>54</v>
+      </c>
+      <c r="S10" s="9" t="s">
+        <v>53</v>
+      </c>
+      <c r="T10" s="9" t="s">
+        <v>52</v>
+      </c>
+      <c r="U10" s="14" t="s">
         <v>51</v>
-      </c>
-      <c r="G10" s="9" t="s">
-        <v>50</v>
-      </c>
-      <c r="H10" s="9" t="s">
-        <v>49</v>
-      </c>
-      <c r="I10" s="22" t="s">
-        <v>48</v>
-      </c>
-      <c r="J10" s="12" t="s">
-        <v>47</v>
-      </c>
-      <c r="K10" s="9" t="s">
-        <v>46</v>
-      </c>
-      <c r="L10" s="9" t="s">
-        <v>45</v>
-      </c>
-      <c r="M10" s="10" t="s">
-        <v>44</v>
-      </c>
-      <c r="N10" s="12" t="s">
-        <v>43</v>
-      </c>
-      <c r="O10" s="12" t="s">
-        <v>42</v>
-      </c>
-      <c r="P10" s="12" t="s">
-        <v>41</v>
-      </c>
-      <c r="Q10" s="22" t="s">
-        <v>40</v>
-      </c>
-      <c r="R10" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="S10" s="9" t="s">
-        <v>38</v>
-      </c>
-      <c r="T10" s="9" t="s">
-        <v>37</v>
-      </c>
-      <c r="U10" s="14" t="s">
-        <v>36</v>
       </c>
     </row>
     <row r="11" spans="2:21" ht="67.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B11" s="6" t="s">
-        <v>52</v>
-      </c>
-      <c r="C11" s="18">
+        <v>67</v>
+      </c>
+      <c r="C11" s="17">
         <v>16</v>
       </c>
-      <c r="D11" s="19">
+      <c r="D11" s="18">
         <v>171</v>
       </c>
       <c r="E11" s="7" t="s">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="F11" s="8"/>
       <c r="G11" s="9"/>
       <c r="H11" s="9"/>
       <c r="I11" s="10" t="s">
-        <v>64</v>
+        <v>79</v>
       </c>
       <c r="J11" s="12" t="s">
-        <v>63</v>
+        <v>78</v>
       </c>
       <c r="K11" s="9" t="s">
-        <v>62</v>
+        <v>77</v>
       </c>
       <c r="L11" s="9" t="s">
-        <v>61</v>
+        <v>76</v>
       </c>
       <c r="M11" s="10" t="s">
-        <v>60</v>
+        <v>75</v>
       </c>
       <c r="N11" s="12" t="s">
-        <v>59</v>
+        <v>74</v>
       </c>
       <c r="O11" s="12" t="s">
-        <v>58</v>
+        <v>73</v>
       </c>
       <c r="P11" s="12" t="s">
-        <v>57</v>
-      </c>
-      <c r="Q11" s="22" t="s">
-        <v>56</v>
+        <v>72</v>
+      </c>
+      <c r="Q11" s="21" t="s">
+        <v>71</v>
       </c>
       <c r="R11" s="12" t="s">
-        <v>55</v>
+        <v>70</v>
       </c>
       <c r="S11" s="9" t="s">
-        <v>54</v>
+        <v>69</v>
       </c>
       <c r="T11" s="9" t="s">
-        <v>54</v>
+        <v>69</v>
       </c>
       <c r="U11" s="14" t="s">
-        <v>53</v>
+        <v>68</v>
       </c>
     </row>
     <row r="12" spans="2:21" ht="67.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B12" s="6" t="s">
-        <v>77</v>
-      </c>
-      <c r="C12" s="18">
+        <v>92</v>
+      </c>
+      <c r="C12" s="17">
         <v>16</v>
       </c>
-      <c r="D12" s="19">
+      <c r="D12" s="18">
         <v>207</v>
       </c>
       <c r="E12" s="7" t="s">
-        <v>65</v>
+        <v>80</v>
       </c>
       <c r="F12" s="33" t="s">
-        <v>76</v>
+        <v>91</v>
       </c>
       <c r="G12" s="34"/>
       <c r="H12" s="49"/>
@@ -2240,305 +2534,305 @@
       <c r="J12" s="12"/>
       <c r="K12" s="12"/>
       <c r="L12" s="9" t="s">
-        <v>75</v>
+        <v>90</v>
       </c>
       <c r="M12" s="10" t="s">
-        <v>74</v>
+        <v>89</v>
       </c>
       <c r="N12" s="12" t="s">
-        <v>73</v>
+        <v>88</v>
       </c>
       <c r="O12" s="12" t="s">
-        <v>72</v>
+        <v>87</v>
       </c>
       <c r="P12" s="12" t="s">
-        <v>71</v>
-      </c>
-      <c r="Q12" s="22" t="s">
-        <v>70</v>
+        <v>86</v>
+      </c>
+      <c r="Q12" s="21" t="s">
+        <v>85</v>
       </c>
       <c r="R12" s="12" t="s">
-        <v>69</v>
+        <v>84</v>
       </c>
       <c r="S12" s="9" t="s">
-        <v>68</v>
+        <v>83</v>
       </c>
       <c r="T12" s="50" t="s">
-        <v>67</v>
+        <v>82</v>
       </c>
       <c r="U12" s="14" t="s">
-        <v>66</v>
+        <v>81</v>
       </c>
     </row>
     <row r="13" spans="2:21" ht="67.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B13" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="C13" s="18">
+        <v>93</v>
+      </c>
+      <c r="C13" s="17">
         <v>16</v>
       </c>
-      <c r="D13" s="19">
+      <c r="D13" s="18">
         <v>211</v>
       </c>
       <c r="E13" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="F13" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="G13" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="H13" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="I13" s="19" t="s">
-        <v>19</v>
+        <v>22</v>
+      </c>
+      <c r="F13" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="G13" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="H13" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="I13" s="18" t="s">
+        <v>34</v>
       </c>
       <c r="J13" s="9" t="s">
-        <v>95</v>
+        <v>110</v>
       </c>
       <c r="K13" s="9" t="s">
-        <v>96</v>
+        <v>111</v>
       </c>
       <c r="L13" s="8" t="s">
-        <v>94</v>
+        <v>109</v>
       </c>
       <c r="M13" s="12" t="s">
-        <v>93</v>
+        <v>108</v>
       </c>
       <c r="N13" s="8" t="s">
-        <v>91</v>
+        <v>106</v>
       </c>
       <c r="O13" s="12" t="s">
-        <v>92</v>
+        <v>107</v>
       </c>
       <c r="P13" s="8" t="s">
-        <v>89</v>
+        <v>104</v>
       </c>
       <c r="Q13" s="12" t="s">
-        <v>90</v>
+        <v>105</v>
       </c>
       <c r="R13" s="8" t="s">
-        <v>88</v>
+        <v>103</v>
       </c>
       <c r="S13" s="10" t="s">
-        <v>87</v>
+        <v>102</v>
       </c>
       <c r="T13" s="12" t="s">
-        <v>86</v>
+        <v>101</v>
       </c>
       <c r="U13" s="14" t="s">
-        <v>85</v>
+        <v>100</v>
       </c>
     </row>
     <row r="14" spans="2:21" ht="67.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B14" s="6" t="s">
+        <v>112</v>
+      </c>
+      <c r="C14" s="17">
+        <v>16</v>
+      </c>
+      <c r="D14" s="18">
+        <v>213</v>
+      </c>
+      <c r="E14" s="7" t="s">
+        <v>35</v>
+      </c>
+      <c r="F14" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="G14" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="H14" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="I14" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="J14" s="9" t="s">
+        <v>117</v>
+      </c>
+      <c r="K14" s="9" t="s">
+        <v>118</v>
+      </c>
+      <c r="L14" s="8" t="s">
+        <v>115</v>
+      </c>
+      <c r="M14" s="9" t="s">
+        <v>116</v>
+      </c>
+      <c r="N14" s="8" t="s">
+        <v>113</v>
+      </c>
+      <c r="O14" s="9" t="s">
+        <v>114</v>
+      </c>
+      <c r="P14" s="8" t="s">
+        <v>99</v>
+      </c>
+      <c r="Q14" s="9" t="s">
+        <v>98</v>
+      </c>
+      <c r="R14" s="8" t="s">
         <v>97</v>
       </c>
-      <c r="C14" s="18">
-        <v>16</v>
-      </c>
-      <c r="D14" s="19">
-        <v>213</v>
-      </c>
-      <c r="E14" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="F14" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="G14" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="H14" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="I14" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="J14" s="9" t="s">
-        <v>102</v>
-      </c>
-      <c r="K14" s="9" t="s">
-        <v>103</v>
-      </c>
-      <c r="L14" s="8" t="s">
-        <v>100</v>
-      </c>
-      <c r="M14" s="9" t="s">
-        <v>101</v>
-      </c>
-      <c r="N14" s="8" t="s">
-        <v>98</v>
-      </c>
-      <c r="O14" s="9" t="s">
-        <v>99</v>
-      </c>
-      <c r="P14" s="8" t="s">
-        <v>84</v>
-      </c>
-      <c r="Q14" s="9" t="s">
-        <v>83</v>
-      </c>
-      <c r="R14" s="8" t="s">
-        <v>82</v>
-      </c>
       <c r="S14" s="10" t="s">
-        <v>81</v>
+        <v>96</v>
       </c>
       <c r="T14" s="9" t="s">
-        <v>80</v>
+        <v>95</v>
       </c>
       <c r="U14" s="14" t="s">
-        <v>79</v>
+        <v>94</v>
       </c>
     </row>
     <row r="15" spans="2:21" ht="67.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B15" s="6" t="s">
-        <v>104</v>
-      </c>
-      <c r="C15" s="18">
+        <v>119</v>
+      </c>
+      <c r="C15" s="17">
         <v>16</v>
       </c>
-      <c r="D15" s="19">
+      <c r="D15" s="18">
         <v>215</v>
       </c>
       <c r="E15" s="7" t="s">
-        <v>20</v>
+        <v>35</v>
       </c>
       <c r="F15" s="8" t="s">
-        <v>116</v>
+        <v>131</v>
       </c>
       <c r="G15" s="9" t="s">
-        <v>117</v>
+        <v>132</v>
       </c>
       <c r="H15" s="8" t="s">
-        <v>118</v>
+        <v>133</v>
       </c>
       <c r="I15" s="8" t="s">
-        <v>115</v>
+        <v>130</v>
       </c>
       <c r="J15" s="9" t="s">
-        <v>114</v>
+        <v>129</v>
       </c>
       <c r="K15" s="8" t="s">
-        <v>113</v>
+        <v>128</v>
       </c>
       <c r="L15" s="8" t="s">
-        <v>112</v>
+        <v>127</v>
       </c>
       <c r="M15" s="9" t="s">
-        <v>111</v>
+        <v>126</v>
       </c>
       <c r="N15" s="8" t="s">
-        <v>110</v>
+        <v>125</v>
       </c>
       <c r="O15" s="9" t="s">
-        <v>109</v>
+        <v>124</v>
       </c>
       <c r="P15" s="8" t="s">
-        <v>108</v>
+        <v>123</v>
       </c>
       <c r="Q15" s="9" t="s">
-        <v>107</v>
+        <v>122</v>
       </c>
       <c r="R15" s="8" t="s">
-        <v>106</v>
+        <v>121</v>
       </c>
       <c r="S15" s="10" t="s">
-        <v>105</v>
+        <v>120</v>
       </c>
       <c r="T15" s="12" t="s">
-        <v>55</v>
+        <v>70</v>
       </c>
       <c r="U15" s="14" t="s">
-        <v>54</v>
+        <v>69</v>
       </c>
     </row>
     <row r="16" spans="2:21" ht="67.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B16" s="6" t="s">
-        <v>119</v>
-      </c>
-      <c r="C16" s="18">
+        <v>134</v>
+      </c>
+      <c r="C16" s="17">
         <v>16</v>
       </c>
-      <c r="D16" s="19">
+      <c r="D16" s="18">
         <v>217</v>
       </c>
       <c r="E16" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="F16" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="G16" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="H16" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="I16" s="19" t="s">
-        <v>19</v>
+        <v>35</v>
+      </c>
+      <c r="F16" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="G16" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="H16" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="I16" s="18" t="s">
+        <v>34</v>
       </c>
       <c r="J16" s="29" t="s">
-        <v>19</v>
-      </c>
-      <c r="K16" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="L16" s="19" t="s">
-        <v>19</v>
+        <v>34</v>
+      </c>
+      <c r="K16" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="L16" s="18" t="s">
+        <v>34</v>
       </c>
       <c r="M16" s="8" t="s">
-        <v>128</v>
+        <v>143</v>
       </c>
       <c r="N16" s="9" t="s">
-        <v>127</v>
+        <v>142</v>
       </c>
       <c r="O16" s="8" t="s">
-        <v>126</v>
+        <v>141</v>
       </c>
       <c r="P16" s="8" t="s">
-        <v>125</v>
+        <v>140</v>
       </c>
       <c r="Q16" s="9" t="s">
-        <v>124</v>
+        <v>139</v>
       </c>
       <c r="R16" s="8" t="s">
-        <v>123</v>
+        <v>138</v>
       </c>
       <c r="S16" s="8" t="s">
-        <v>122</v>
+        <v>137</v>
       </c>
       <c r="T16" s="9" t="s">
-        <v>121</v>
+        <v>136</v>
       </c>
       <c r="U16" s="8" t="s">
-        <v>120</v>
+        <v>135</v>
       </c>
     </row>
     <row r="17" spans="2:21" ht="67.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B17" s="23"/>
-      <c r="C17" s="24"/>
-      <c r="D17" s="24"/>
-      <c r="E17" s="25"/>
-      <c r="F17" s="24"/>
-      <c r="G17" s="24"/>
-      <c r="H17" s="24"/>
-      <c r="I17" s="24"/>
-      <c r="J17" s="24"/>
-      <c r="K17" s="24"/>
-      <c r="L17" s="24"/>
-      <c r="M17" s="23"/>
-      <c r="N17" s="23"/>
-      <c r="O17" s="23"/>
-      <c r="P17" s="23"/>
-      <c r="Q17" s="23"/>
-      <c r="R17" s="23"/>
-      <c r="S17" s="23"/>
-      <c r="T17" s="23"/>
-      <c r="U17" s="23"/>
+      <c r="B17" s="22"/>
+      <c r="C17" s="23"/>
+      <c r="D17" s="23"/>
+      <c r="E17" s="24"/>
+      <c r="F17" s="23"/>
+      <c r="G17" s="23"/>
+      <c r="H17" s="23"/>
+      <c r="I17" s="23"/>
+      <c r="J17" s="23"/>
+      <c r="K17" s="23"/>
+      <c r="L17" s="23"/>
+      <c r="M17" s="22"/>
+      <c r="N17" s="22"/>
+      <c r="O17" s="22"/>
+      <c r="P17" s="22"/>
+      <c r="Q17" s="22"/>
+      <c r="R17" s="22"/>
+      <c r="S17" s="22"/>
+      <c r="T17" s="22"/>
+      <c r="U17" s="22"/>
     </row>
     <row r="18" spans="2:21" ht="15.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B18" s="35" t="s">
@@ -2577,262 +2871,262 @@
       <c r="C19" s="38"/>
       <c r="D19" s="40"/>
       <c r="E19" s="42"/>
-      <c r="F19" s="18">
+      <c r="F19" s="17">
         <v>15</v>
       </c>
-      <c r="G19" s="19">
+      <c r="G19" s="18">
         <v>14</v>
       </c>
-      <c r="H19" s="19">
+      <c r="H19" s="18">
         <v>13</v>
       </c>
-      <c r="I19" s="20">
+      <c r="I19" s="19">
         <v>12</v>
       </c>
-      <c r="J19" s="18">
+      <c r="J19" s="17">
         <v>11</v>
       </c>
-      <c r="K19" s="19">
+      <c r="K19" s="18">
         <v>10</v>
       </c>
-      <c r="L19" s="19">
+      <c r="L19" s="18">
         <v>9</v>
       </c>
-      <c r="M19" s="19">
+      <c r="M19" s="18">
         <v>8</v>
       </c>
       <c r="N19" s="29">
         <v>7</v>
       </c>
-      <c r="O19" s="19">
+      <c r="O19" s="18">
         <v>6</v>
       </c>
-      <c r="P19" s="19">
+      <c r="P19" s="18">
         <v>5</v>
       </c>
-      <c r="Q19" s="20">
+      <c r="Q19" s="19">
         <v>4</v>
       </c>
       <c r="R19" s="29">
         <v>3</v>
       </c>
-      <c r="S19" s="19">
+      <c r="S19" s="18">
         <v>2</v>
       </c>
-      <c r="T19" s="19">
+      <c r="T19" s="18">
         <v>1</v>
       </c>
-      <c r="U19" s="20">
+      <c r="U19" s="19">
         <v>0</v>
       </c>
     </row>
     <row r="20" spans="2:21" ht="67.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B20" s="6" t="s">
-        <v>129</v>
-      </c>
-      <c r="C20" s="18">
+        <v>144</v>
+      </c>
+      <c r="C20" s="17">
         <v>16</v>
       </c>
-      <c r="D20" s="19">
+      <c r="D20" s="18">
         <v>342</v>
       </c>
       <c r="E20" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="F20" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="G20" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="H20" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="I20" s="19" t="s">
-        <v>19</v>
+        <v>22</v>
+      </c>
+      <c r="F20" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="G20" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="H20" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="I20" s="18" t="s">
+        <v>34</v>
       </c>
       <c r="J20" s="29" t="s">
-        <v>19</v>
-      </c>
-      <c r="K20" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="L20" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="M20" s="19" t="s">
-        <v>19</v>
+        <v>34</v>
+      </c>
+      <c r="K20" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="L20" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="M20" s="18" t="s">
+        <v>34</v>
       </c>
       <c r="N20" s="9" t="s">
-        <v>137</v>
+        <v>152</v>
       </c>
       <c r="O20" s="9" t="s">
-        <v>136</v>
+        <v>151</v>
       </c>
       <c r="P20" s="9" t="s">
-        <v>135</v>
+        <v>150</v>
       </c>
       <c r="Q20" s="9" t="s">
-        <v>134</v>
+        <v>149</v>
       </c>
       <c r="R20" s="9" t="s">
-        <v>133</v>
+        <v>148</v>
       </c>
       <c r="S20" s="9" t="s">
-        <v>132</v>
+        <v>147</v>
       </c>
       <c r="T20" s="9" t="s">
-        <v>131</v>
+        <v>146</v>
       </c>
       <c r="U20" s="14" t="s">
-        <v>130</v>
+        <v>145</v>
       </c>
     </row>
     <row r="21" spans="2:21" ht="67.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B21" s="6" t="s">
-        <v>138</v>
-      </c>
-      <c r="C21" s="18">
+        <v>153</v>
+      </c>
+      <c r="C21" s="17">
         <v>16</v>
       </c>
-      <c r="D21" s="19">
+      <c r="D21" s="18">
         <v>344</v>
       </c>
       <c r="E21" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="F21" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="G21" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="H21" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="I21" s="19" t="s">
-        <v>19</v>
+        <v>35</v>
+      </c>
+      <c r="F21" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="G21" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="H21" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="I21" s="18" t="s">
+        <v>34</v>
       </c>
       <c r="J21" s="29" t="s">
-        <v>19</v>
-      </c>
-      <c r="K21" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="L21" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="M21" s="19" t="s">
-        <v>19</v>
+        <v>34</v>
+      </c>
+      <c r="K21" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="L21" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="M21" s="18" t="s">
+        <v>34</v>
       </c>
       <c r="N21" s="9" t="s">
-        <v>146</v>
+        <v>161</v>
       </c>
       <c r="O21" s="9" t="s">
-        <v>145</v>
+        <v>160</v>
       </c>
       <c r="P21" s="9" t="s">
-        <v>144</v>
+        <v>159</v>
       </c>
       <c r="Q21" s="9" t="s">
-        <v>143</v>
+        <v>158</v>
       </c>
       <c r="R21" s="9" t="s">
-        <v>142</v>
+        <v>157</v>
       </c>
       <c r="S21" s="9" t="s">
-        <v>141</v>
+        <v>156</v>
       </c>
       <c r="T21" s="9" t="s">
-        <v>140</v>
+        <v>155</v>
       </c>
       <c r="U21" s="14" t="s">
-        <v>139</v>
+        <v>154</v>
       </c>
     </row>
     <row r="22" spans="2:21" ht="67.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B22" s="6" t="s">
-        <v>147</v>
-      </c>
-      <c r="C22" s="18">
+        <v>162</v>
+      </c>
+      <c r="C22" s="17">
         <v>16</v>
       </c>
-      <c r="D22" s="19">
+      <c r="D22" s="18">
         <v>346</v>
       </c>
       <c r="E22" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="F22" s="18" t="s">
-        <v>19</v>
+        <v>35</v>
+      </c>
+      <c r="F22" s="17" t="s">
+        <v>34</v>
       </c>
       <c r="G22" s="8" t="s">
-        <v>158</v>
+        <v>173</v>
       </c>
       <c r="H22" s="8" t="s">
-        <v>157</v>
+        <v>172</v>
       </c>
       <c r="I22" s="8" t="s">
-        <v>156</v>
+        <v>171</v>
       </c>
       <c r="J22" s="8" t="s">
-        <v>155</v>
+        <v>170</v>
       </c>
       <c r="K22" s="8" t="s">
-        <v>154</v>
+        <v>169</v>
       </c>
       <c r="L22" s="8" t="s">
-        <v>153</v>
+        <v>168</v>
       </c>
       <c r="M22" s="9" t="s">
-        <v>109</v>
+        <v>124</v>
       </c>
       <c r="N22" s="8" t="s">
-        <v>108</v>
+        <v>123</v>
       </c>
       <c r="O22" s="9" t="s">
-        <v>107</v>
+        <v>122</v>
       </c>
       <c r="P22" s="8" t="s">
-        <v>106</v>
+        <v>121</v>
       </c>
       <c r="Q22" s="9" t="s">
-        <v>152</v>
+        <v>167</v>
       </c>
       <c r="R22" s="8" t="s">
-        <v>151</v>
+        <v>166</v>
       </c>
       <c r="S22" s="10" t="s">
-        <v>150</v>
+        <v>165</v>
       </c>
       <c r="T22" s="12" t="s">
-        <v>149</v>
+        <v>164</v>
       </c>
       <c r="U22" s="14" t="s">
-        <v>148</v>
+        <v>163</v>
       </c>
     </row>
     <row r="23" spans="2:21" ht="67.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B23" s="23"/>
-      <c r="C23" s="24"/>
-      <c r="D23" s="24"/>
-      <c r="E23" s="25"/>
-      <c r="F23" s="24"/>
-      <c r="G23" s="24"/>
-      <c r="H23" s="24"/>
-      <c r="I23" s="24"/>
-      <c r="J23" s="24"/>
-      <c r="K23" s="24"/>
-      <c r="L23" s="24"/>
-      <c r="M23" s="23"/>
-      <c r="N23" s="23"/>
-      <c r="O23" s="23"/>
-      <c r="P23" s="23"/>
-      <c r="Q23" s="23"/>
-      <c r="R23" s="23"/>
-      <c r="S23" s="23"/>
-      <c r="T23" s="23"/>
-      <c r="U23" s="23"/>
+      <c r="B23" s="22"/>
+      <c r="C23" s="23"/>
+      <c r="D23" s="23"/>
+      <c r="E23" s="24"/>
+      <c r="F23" s="23"/>
+      <c r="G23" s="23"/>
+      <c r="H23" s="23"/>
+      <c r="I23" s="23"/>
+      <c r="J23" s="23"/>
+      <c r="K23" s="23"/>
+      <c r="L23" s="23"/>
+      <c r="M23" s="22"/>
+      <c r="N23" s="22"/>
+      <c r="O23" s="22"/>
+      <c r="P23" s="22"/>
+      <c r="Q23" s="22"/>
+      <c r="R23" s="22"/>
+      <c r="S23" s="22"/>
+      <c r="T23" s="22"/>
+      <c r="U23" s="22"/>
     </row>
     <row r="24" spans="2:21" ht="16.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B24" s="35" t="s">
@@ -2857,14 +3151,14 @@
       <c r="K24" s="44"/>
       <c r="L24" s="44"/>
       <c r="M24" s="48"/>
-      <c r="N24" s="23"/>
-      <c r="O24" s="23"/>
-      <c r="P24" s="23"/>
-      <c r="Q24" s="23"/>
-      <c r="R24" s="23"/>
-      <c r="S24" s="23"/>
-      <c r="T24" s="23"/>
-      <c r="U24" s="23"/>
+      <c r="N24" s="22"/>
+      <c r="O24" s="22"/>
+      <c r="P24" s="22"/>
+      <c r="Q24" s="22"/>
+      <c r="R24" s="22"/>
+      <c r="S24" s="22"/>
+      <c r="T24" s="22"/>
+      <c r="U24" s="22"/>
     </row>
     <row r="25" spans="2:21" ht="16.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B25" s="36"/>
@@ -2883,7 +3177,7 @@
       <c r="I25" s="32">
         <v>4</v>
       </c>
-      <c r="J25" s="16">
+      <c r="J25" s="15">
         <v>3</v>
       </c>
       <c r="K25" s="31">
@@ -2895,124 +3189,124 @@
       <c r="M25" s="32">
         <v>0</v>
       </c>
-      <c r="N25" s="23"/>
-      <c r="O25" s="23"/>
-      <c r="P25" s="23"/>
-      <c r="Q25" s="23"/>
-      <c r="R25" s="23"/>
-      <c r="S25" s="23"/>
-      <c r="T25" s="23"/>
-      <c r="U25" s="23"/>
+      <c r="N25" s="22"/>
+      <c r="O25" s="22"/>
+      <c r="P25" s="22"/>
+      <c r="Q25" s="22"/>
+      <c r="R25" s="22"/>
+      <c r="S25" s="22"/>
+      <c r="T25" s="22"/>
+      <c r="U25" s="22"/>
     </row>
     <row r="26" spans="2:21" ht="67.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B26" s="6" t="s">
-        <v>165</v>
-      </c>
-      <c r="C26" s="18">
+        <v>180</v>
+      </c>
+      <c r="C26" s="17">
         <v>8</v>
       </c>
-      <c r="D26" s="19">
+      <c r="D26" s="18">
         <v>355</v>
       </c>
       <c r="E26" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="F26" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="G26" s="19" t="s">
-        <v>19</v>
+        <v>22</v>
+      </c>
+      <c r="F26" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="G26" s="18" t="s">
+        <v>34</v>
       </c>
       <c r="H26" s="12" t="s">
-        <v>164</v>
+        <v>179</v>
       </c>
       <c r="I26" s="13" t="s">
-        <v>163</v>
-      </c>
-      <c r="J26" s="17" t="s">
-        <v>162</v>
+        <v>178</v>
+      </c>
+      <c r="J26" s="16" t="s">
+        <v>177</v>
       </c>
       <c r="K26" s="12" t="s">
-        <v>161</v>
+        <v>176</v>
       </c>
       <c r="L26" s="12" t="s">
-        <v>160</v>
+        <v>175</v>
       </c>
       <c r="M26" s="13" t="s">
-        <v>159</v>
-      </c>
-      <c r="N26" s="23"/>
-      <c r="O26" s="23"/>
-      <c r="P26" s="23"/>
-      <c r="Q26" s="23"/>
-      <c r="R26" s="23"/>
-      <c r="S26" s="23"/>
-      <c r="T26" s="23"/>
-      <c r="U26" s="23"/>
+        <v>174</v>
+      </c>
+      <c r="N26" s="22"/>
+      <c r="O26" s="22"/>
+      <c r="P26" s="22"/>
+      <c r="Q26" s="22"/>
+      <c r="R26" s="22"/>
+      <c r="S26" s="22"/>
+      <c r="T26" s="22"/>
+      <c r="U26" s="22"/>
     </row>
     <row r="27" spans="2:21" ht="67.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B27" s="6" t="s">
-        <v>166</v>
-      </c>
-      <c r="C27" s="18">
+        <v>181</v>
+      </c>
+      <c r="C27" s="17">
         <v>8</v>
       </c>
-      <c r="D27" s="19">
+      <c r="D27" s="18">
         <v>356</v>
       </c>
       <c r="E27" s="7" t="s">
-        <v>20</v>
-      </c>
-      <c r="F27" s="18"/>
-      <c r="G27" s="19"/>
+        <v>35</v>
+      </c>
+      <c r="F27" s="17"/>
+      <c r="G27" s="18"/>
       <c r="H27" s="13" t="s">
-        <v>172</v>
+        <v>187</v>
       </c>
       <c r="I27" s="13" t="s">
-        <v>171</v>
+        <v>186</v>
       </c>
       <c r="J27" s="13" t="s">
-        <v>170</v>
+        <v>185</v>
       </c>
       <c r="K27" s="13" t="s">
-        <v>169</v>
+        <v>184</v>
       </c>
       <c r="L27" s="13" t="s">
-        <v>168</v>
+        <v>183</v>
       </c>
       <c r="M27" s="13" t="s">
-        <v>167</v>
-      </c>
-      <c r="N27" s="23"/>
-      <c r="O27" s="23"/>
-      <c r="P27" s="23"/>
-      <c r="Q27" s="23"/>
-      <c r="R27" s="23"/>
-      <c r="S27" s="23"/>
-      <c r="T27" s="23"/>
-      <c r="U27" s="23"/>
+        <v>182</v>
+      </c>
+      <c r="N27" s="22"/>
+      <c r="O27" s="22"/>
+      <c r="P27" s="22"/>
+      <c r="Q27" s="22"/>
+      <c r="R27" s="22"/>
+      <c r="S27" s="22"/>
+      <c r="T27" s="22"/>
+      <c r="U27" s="22"/>
     </row>
     <row r="28" spans="2:21" ht="67.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B28" s="23"/>
-      <c r="C28" s="24"/>
-      <c r="D28" s="24"/>
-      <c r="E28" s="25"/>
-      <c r="F28" s="24"/>
-      <c r="G28" s="24"/>
-      <c r="H28" s="23"/>
-      <c r="I28" s="23"/>
-      <c r="J28" s="23"/>
-      <c r="K28" s="23"/>
-      <c r="L28" s="23"/>
-      <c r="M28" s="23"/>
-      <c r="N28" s="23"/>
-      <c r="O28" s="23"/>
-      <c r="P28" s="23"/>
-      <c r="Q28" s="23"/>
-      <c r="R28" s="23"/>
-      <c r="S28" s="23"/>
-      <c r="T28" s="23"/>
-      <c r="U28" s="23"/>
+      <c r="B28" s="22"/>
+      <c r="C28" s="23"/>
+      <c r="D28" s="23"/>
+      <c r="E28" s="24"/>
+      <c r="F28" s="23"/>
+      <c r="G28" s="23"/>
+      <c r="H28" s="22"/>
+      <c r="I28" s="22"/>
+      <c r="J28" s="22"/>
+      <c r="K28" s="22"/>
+      <c r="L28" s="22"/>
+      <c r="M28" s="22"/>
+      <c r="N28" s="22"/>
+      <c r="O28" s="22"/>
+      <c r="P28" s="22"/>
+      <c r="Q28" s="22"/>
+      <c r="R28" s="22"/>
+      <c r="S28" s="22"/>
+      <c r="T28" s="22"/>
+      <c r="U28" s="22"/>
     </row>
     <row r="29" spans="2:21" ht="17.399999999999999" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B29" s="35" t="s">
@@ -3051,31 +3345,31 @@
       <c r="C30" s="38"/>
       <c r="D30" s="40"/>
       <c r="E30" s="42"/>
-      <c r="F30" s="18">
+      <c r="F30" s="17">
         <v>15</v>
       </c>
-      <c r="G30" s="19">
+      <c r="G30" s="18">
         <v>14</v>
       </c>
-      <c r="H30" s="19">
+      <c r="H30" s="18">
         <v>13</v>
       </c>
-      <c r="I30" s="20">
+      <c r="I30" s="19">
         <v>12</v>
       </c>
-      <c r="J30" s="18">
+      <c r="J30" s="17">
         <v>11</v>
       </c>
-      <c r="K30" s="19">
+      <c r="K30" s="18">
         <v>10</v>
       </c>
-      <c r="L30" s="19">
+      <c r="L30" s="18">
         <v>9</v>
       </c>
-      <c r="M30" s="19">
+      <c r="M30" s="18">
         <v>8</v>
       </c>
-      <c r="N30" s="16">
+      <c r="N30" s="15">
         <v>7</v>
       </c>
       <c r="O30" s="31">
@@ -3087,413 +3381,413 @@
       <c r="Q30" s="32">
         <v>4</v>
       </c>
-      <c r="R30" s="16">
+      <c r="R30" s="15">
         <v>3</v>
       </c>
       <c r="S30" s="31">
         <v>2</v>
       </c>
-      <c r="T30" s="19">
+      <c r="T30" s="18">
         <v>1</v>
       </c>
-      <c r="U30" s="20">
+      <c r="U30" s="19">
         <v>0</v>
       </c>
     </row>
     <row r="31" spans="2:21" ht="67.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B31" s="6" t="s">
-        <v>173</v>
-      </c>
-      <c r="C31" s="18">
+        <v>188</v>
+      </c>
+      <c r="C31" s="17">
         <v>16</v>
       </c>
-      <c r="D31" s="19">
+      <c r="D31" s="18">
         <v>381</v>
       </c>
       <c r="E31" s="7" t="s">
-        <v>182</v>
-      </c>
-      <c r="F31" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="G31" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="H31" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="I31" s="19" t="s">
-        <v>19</v>
+        <v>197</v>
+      </c>
+      <c r="F31" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="G31" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="H31" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="I31" s="18" t="s">
+        <v>34</v>
       </c>
       <c r="J31" s="9" t="s">
-        <v>186</v>
+        <v>201</v>
       </c>
       <c r="K31" s="9" t="s">
-        <v>185</v>
+        <v>200</v>
       </c>
       <c r="L31" s="9" t="s">
-        <v>184</v>
-      </c>
-      <c r="M31" s="22" t="s">
-        <v>183</v>
+        <v>199</v>
+      </c>
+      <c r="M31" s="21" t="s">
+        <v>198</v>
       </c>
       <c r="N31" s="11" t="s">
-        <v>181</v>
-      </c>
-      <c r="O31" s="28" t="s">
-        <v>180</v>
-      </c>
-      <c r="P31" s="22" t="s">
-        <v>179</v>
-      </c>
-      <c r="Q31" s="22" t="s">
-        <v>178</v>
-      </c>
-      <c r="R31" s="22" t="s">
-        <v>177</v>
+        <v>196</v>
+      </c>
+      <c r="O31" s="27" t="s">
+        <v>195</v>
+      </c>
+      <c r="P31" s="21" t="s">
+        <v>194</v>
+      </c>
+      <c r="Q31" s="21" t="s">
+        <v>193</v>
+      </c>
+      <c r="R31" s="21" t="s">
+        <v>192</v>
       </c>
       <c r="S31" s="12" t="s">
-        <v>176</v>
+        <v>191</v>
       </c>
       <c r="T31" s="8" t="s">
-        <v>175</v>
+        <v>190</v>
       </c>
       <c r="U31" s="14" t="s">
-        <v>174</v>
+        <v>189</v>
       </c>
     </row>
     <row r="32" spans="2:21" ht="67.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B32" s="6" t="s">
-        <v>187</v>
-      </c>
-      <c r="C32" s="18">
+        <v>202</v>
+      </c>
+      <c r="C32" s="17">
         <v>16</v>
       </c>
-      <c r="D32" s="19">
+      <c r="D32" s="18">
         <v>383</v>
       </c>
       <c r="E32" s="7" t="s">
-        <v>182</v>
-      </c>
-      <c r="F32" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="G32" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="H32" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="I32" s="19" t="s">
-        <v>19</v>
+        <v>197</v>
+      </c>
+      <c r="F32" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="G32" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="H32" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="I32" s="18" t="s">
+        <v>34</v>
       </c>
       <c r="J32" s="9" t="s">
-        <v>199</v>
+        <v>214</v>
       </c>
       <c r="K32" s="9" t="s">
-        <v>198</v>
+        <v>213</v>
       </c>
       <c r="L32" s="9" t="s">
-        <v>197</v>
-      </c>
-      <c r="M32" s="22" t="s">
-        <v>196</v>
+        <v>212</v>
+      </c>
+      <c r="M32" s="21" t="s">
+        <v>211</v>
       </c>
       <c r="N32" s="11" t="s">
-        <v>195</v>
-      </c>
-      <c r="O32" s="28" t="s">
-        <v>194</v>
-      </c>
-      <c r="P32" s="22" t="s">
-        <v>193</v>
-      </c>
-      <c r="Q32" s="22" t="s">
-        <v>192</v>
-      </c>
-      <c r="R32" s="22" t="s">
-        <v>191</v>
+        <v>210</v>
+      </c>
+      <c r="O32" s="27" t="s">
+        <v>209</v>
+      </c>
+      <c r="P32" s="21" t="s">
+        <v>208</v>
+      </c>
+      <c r="Q32" s="21" t="s">
+        <v>207</v>
+      </c>
+      <c r="R32" s="21" t="s">
+        <v>206</v>
       </c>
       <c r="S32" s="12" t="s">
-        <v>190</v>
+        <v>205</v>
       </c>
       <c r="T32" s="8" t="s">
-        <v>189</v>
+        <v>204</v>
       </c>
       <c r="U32" s="14" t="s">
-        <v>188</v>
+        <v>203</v>
       </c>
     </row>
     <row r="33" spans="2:21" ht="67.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B33" s="6" t="s">
-        <v>200</v>
-      </c>
-      <c r="C33" s="18">
+        <v>215</v>
+      </c>
+      <c r="C33" s="17">
         <v>16</v>
       </c>
-      <c r="D33" s="19">
+      <c r="D33" s="18">
         <v>385</v>
       </c>
       <c r="E33" s="7" t="s">
-        <v>182</v>
-      </c>
-      <c r="F33" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="G33" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="H33" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="I33" s="19" t="s">
-        <v>19</v>
+        <v>197</v>
+      </c>
+      <c r="F33" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="G33" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="H33" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="I33" s="18" t="s">
+        <v>34</v>
       </c>
       <c r="J33" s="9" t="s">
-        <v>212</v>
+        <v>227</v>
       </c>
       <c r="K33" s="9" t="s">
-        <v>211</v>
+        <v>226</v>
       </c>
       <c r="L33" s="9" t="s">
-        <v>210</v>
-      </c>
-      <c r="M33" s="22" t="s">
-        <v>209</v>
+        <v>225</v>
+      </c>
+      <c r="M33" s="21" t="s">
+        <v>224</v>
       </c>
       <c r="N33" s="11" t="s">
-        <v>208</v>
-      </c>
-      <c r="O33" s="28" t="s">
-        <v>207</v>
-      </c>
-      <c r="P33" s="22" t="s">
-        <v>206</v>
-      </c>
-      <c r="Q33" s="22" t="s">
-        <v>205</v>
-      </c>
-      <c r="R33" s="22" t="s">
-        <v>204</v>
+        <v>223</v>
+      </c>
+      <c r="O33" s="27" t="s">
+        <v>222</v>
+      </c>
+      <c r="P33" s="21" t="s">
+        <v>221</v>
+      </c>
+      <c r="Q33" s="21" t="s">
+        <v>220</v>
+      </c>
+      <c r="R33" s="21" t="s">
+        <v>219</v>
       </c>
       <c r="S33" s="12" t="s">
-        <v>203</v>
+        <v>218</v>
       </c>
       <c r="T33" s="8" t="s">
-        <v>202</v>
+        <v>217</v>
       </c>
       <c r="U33" s="14" t="s">
-        <v>201</v>
+        <v>216</v>
       </c>
     </row>
     <row r="34" spans="2:21" ht="67.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B34" s="6" t="s">
-        <v>213</v>
-      </c>
-      <c r="C34" s="18">
+        <v>228</v>
+      </c>
+      <c r="C34" s="17">
         <v>16</v>
       </c>
-      <c r="D34" s="19">
+      <c r="D34" s="18">
         <v>387</v>
       </c>
       <c r="E34" s="7" t="s">
-        <v>182</v>
-      </c>
-      <c r="F34" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="G34" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="H34" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="I34" s="19" t="s">
-        <v>19</v>
+        <v>197</v>
+      </c>
+      <c r="F34" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="G34" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="H34" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="I34" s="18" t="s">
+        <v>34</v>
       </c>
       <c r="J34" s="9" t="s">
-        <v>225</v>
+        <v>240</v>
       </c>
       <c r="K34" s="9" t="s">
-        <v>224</v>
+        <v>239</v>
       </c>
       <c r="L34" s="9" t="s">
-        <v>223</v>
-      </c>
-      <c r="M34" s="22" t="s">
-        <v>222</v>
+        <v>238</v>
+      </c>
+      <c r="M34" s="21" t="s">
+        <v>237</v>
       </c>
       <c r="N34" s="11" t="s">
-        <v>221</v>
-      </c>
-      <c r="O34" s="28" t="s">
-        <v>220</v>
-      </c>
-      <c r="P34" s="22" t="s">
-        <v>219</v>
-      </c>
-      <c r="Q34" s="22" t="s">
-        <v>218</v>
-      </c>
-      <c r="R34" s="22" t="s">
-        <v>217</v>
+        <v>236</v>
+      </c>
+      <c r="O34" s="27" t="s">
+        <v>235</v>
+      </c>
+      <c r="P34" s="21" t="s">
+        <v>234</v>
+      </c>
+      <c r="Q34" s="21" t="s">
+        <v>233</v>
+      </c>
+      <c r="R34" s="21" t="s">
+        <v>232</v>
       </c>
       <c r="S34" s="12" t="s">
-        <v>216</v>
+        <v>231</v>
       </c>
       <c r="T34" s="8" t="s">
-        <v>215</v>
+        <v>230</v>
       </c>
       <c r="U34" s="14" t="s">
-        <v>214</v>
+        <v>229</v>
       </c>
     </row>
     <row r="35" spans="2:21" ht="67.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B35" s="6" t="s">
-        <v>226</v>
-      </c>
-      <c r="C35" s="18">
+        <v>241</v>
+      </c>
+      <c r="C35" s="17">
         <v>16</v>
       </c>
-      <c r="D35" s="19">
+      <c r="D35" s="18">
         <v>387</v>
       </c>
       <c r="E35" s="7" t="s">
-        <v>182</v>
-      </c>
-      <c r="F35" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="G35" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="H35" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="I35" s="19" t="s">
-        <v>19</v>
+        <v>197</v>
+      </c>
+      <c r="F35" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="G35" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="H35" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="I35" s="18" t="s">
+        <v>34</v>
       </c>
       <c r="J35" s="9" t="s">
+        <v>262</v>
+      </c>
+      <c r="K35" s="9" t="s">
+        <v>261</v>
+      </c>
+      <c r="L35" s="9" t="s">
+        <v>260</v>
+      </c>
+      <c r="M35" s="21" t="s">
+        <v>259</v>
+      </c>
+      <c r="N35" s="11" t="s">
+        <v>249</v>
+      </c>
+      <c r="O35" s="27" t="s">
+        <v>248</v>
+      </c>
+      <c r="P35" s="21" t="s">
         <v>247</v>
       </c>
-      <c r="K35" s="9" t="s">
+      <c r="Q35" s="21" t="s">
         <v>246</v>
       </c>
-      <c r="L35" s="9" t="s">
+      <c r="R35" s="21" t="s">
         <v>245</v>
       </c>
-      <c r="M35" s="22" t="s">
+      <c r="S35" s="12" t="s">
         <v>244</v>
       </c>
-      <c r="N35" s="11" t="s">
-        <v>234</v>
-      </c>
-      <c r="O35" s="28" t="s">
-        <v>233</v>
-      </c>
-      <c r="P35" s="22" t="s">
-        <v>232</v>
-      </c>
-      <c r="Q35" s="22" t="s">
-        <v>231</v>
-      </c>
-      <c r="R35" s="22" t="s">
-        <v>230</v>
-      </c>
-      <c r="S35" s="12" t="s">
-        <v>229</v>
-      </c>
       <c r="T35" s="8" t="s">
-        <v>228</v>
+        <v>243</v>
       </c>
       <c r="U35" s="14" t="s">
-        <v>227</v>
+        <v>242</v>
       </c>
     </row>
     <row r="36" spans="2:21" ht="67.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B36" s="6" t="s">
-        <v>235</v>
-      </c>
-      <c r="C36" s="18">
+        <v>250</v>
+      </c>
+      <c r="C36" s="17">
         <v>16</v>
       </c>
-      <c r="D36" s="19">
+      <c r="D36" s="18">
         <v>391</v>
       </c>
       <c r="E36" s="7" t="s">
-        <v>182</v>
-      </c>
-      <c r="F36" s="18" t="s">
-        <v>19</v>
-      </c>
-      <c r="G36" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="H36" s="19" t="s">
-        <v>19</v>
-      </c>
-      <c r="I36" s="19" t="s">
-        <v>19</v>
+        <v>197</v>
+      </c>
+      <c r="F36" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="G36" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="H36" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="I36" s="18" t="s">
+        <v>34</v>
       </c>
       <c r="J36" s="9" t="s">
+        <v>266</v>
+      </c>
+      <c r="K36" s="9" t="s">
+        <v>265</v>
+      </c>
+      <c r="L36" s="9" t="s">
+        <v>264</v>
+      </c>
+      <c r="M36" s="21" t="s">
+        <v>263</v>
+      </c>
+      <c r="N36" s="11" t="s">
+        <v>258</v>
+      </c>
+      <c r="O36" s="27" t="s">
+        <v>257</v>
+      </c>
+      <c r="P36" s="21" t="s">
+        <v>256</v>
+      </c>
+      <c r="Q36" s="21" t="s">
+        <v>255</v>
+      </c>
+      <c r="R36" s="21" t="s">
+        <v>254</v>
+      </c>
+      <c r="S36" s="12" t="s">
+        <v>253</v>
+      </c>
+      <c r="T36" s="8" t="s">
+        <v>252</v>
+      </c>
+      <c r="U36" s="14" t="s">
         <v>251</v>
-      </c>
-      <c r="K36" s="9" t="s">
-        <v>250</v>
-      </c>
-      <c r="L36" s="9" t="s">
-        <v>249</v>
-      </c>
-      <c r="M36" s="22" t="s">
-        <v>248</v>
-      </c>
-      <c r="N36" s="11" t="s">
-        <v>243</v>
-      </c>
-      <c r="O36" s="28" t="s">
-        <v>242</v>
-      </c>
-      <c r="P36" s="22" t="s">
-        <v>241</v>
-      </c>
-      <c r="Q36" s="22" t="s">
-        <v>240</v>
-      </c>
-      <c r="R36" s="22" t="s">
-        <v>239</v>
-      </c>
-      <c r="S36" s="12" t="s">
-        <v>238</v>
-      </c>
-      <c r="T36" s="8" t="s">
-        <v>237</v>
-      </c>
-      <c r="U36" s="14" t="s">
-        <v>236</v>
       </c>
     </row>
     <row r="37" spans="2:21" ht="67.8" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="38" spans="2:21" ht="67.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B38" s="23"/>
-      <c r="C38" s="24"/>
-      <c r="D38" s="24"/>
-      <c r="E38" s="25"/>
-      <c r="F38" s="23"/>
-      <c r="G38" s="23"/>
-      <c r="H38" s="23"/>
-      <c r="I38" s="23"/>
-      <c r="J38" s="23"/>
-      <c r="K38" s="23"/>
-      <c r="L38" s="23"/>
-      <c r="M38" s="23"/>
-      <c r="N38" s="23"/>
-      <c r="O38" s="23"/>
-      <c r="P38" s="23"/>
-      <c r="Q38" s="23"/>
-      <c r="R38" s="23"/>
-      <c r="S38" s="23"/>
-      <c r="T38" s="23"/>
-      <c r="U38" s="23"/>
+      <c r="B38" s="22"/>
+      <c r="C38" s="23"/>
+      <c r="D38" s="23"/>
+      <c r="E38" s="24"/>
+      <c r="F38" s="22"/>
+      <c r="G38" s="22"/>
+      <c r="H38" s="22"/>
+      <c r="I38" s="22"/>
+      <c r="J38" s="22"/>
+      <c r="K38" s="22"/>
+      <c r="L38" s="22"/>
+      <c r="M38" s="22"/>
+      <c r="N38" s="22"/>
+      <c r="O38" s="22"/>
+      <c r="P38" s="22"/>
+      <c r="Q38" s="22"/>
+      <c r="R38" s="22"/>
+      <c r="S38" s="22"/>
+      <c r="T38" s="22"/>
+      <c r="U38" s="22"/>
     </row>
     <row r="39" spans="2:21" ht="67.8" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B39" s="35" t="s">
@@ -3532,400 +3826,1363 @@
       <c r="C40" s="38"/>
       <c r="D40" s="40"/>
       <c r="E40" s="42"/>
-      <c r="F40" s="18">
+      <c r="F40" s="17">
         <v>15</v>
       </c>
-      <c r="G40" s="19">
+      <c r="G40" s="18">
         <v>14</v>
       </c>
-      <c r="H40" s="19">
+      <c r="H40" s="18">
         <v>13</v>
       </c>
       <c r="I40" s="4">
         <v>12</v>
       </c>
-      <c r="J40" s="19">
+      <c r="J40" s="18">
         <v>11</v>
       </c>
-      <c r="K40" s="19">
+      <c r="K40" s="18">
         <v>10</v>
       </c>
-      <c r="L40" s="19">
+      <c r="L40" s="18">
         <v>9</v>
       </c>
       <c r="M40" s="4">
         <v>8</v>
       </c>
-      <c r="N40" s="18">
+      <c r="N40" s="17">
         <v>7</v>
       </c>
-      <c r="O40" s="19">
+      <c r="O40" s="18">
         <v>6</v>
       </c>
-      <c r="P40" s="19">
+      <c r="P40" s="18">
         <v>5</v>
       </c>
       <c r="Q40" s="4">
         <v>4</v>
       </c>
-      <c r="R40" s="19">
+      <c r="R40" s="18">
         <v>3</v>
       </c>
       <c r="S40" s="4">
         <v>2</v>
       </c>
-      <c r="T40" s="19">
+      <c r="T40" s="18">
         <v>1</v>
       </c>
-      <c r="U40" s="20">
+      <c r="U40" s="19">
         <v>0</v>
       </c>
     </row>
     <row r="41" spans="2:21" ht="58.2" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B41" s="6" t="s">
-        <v>78</v>
-      </c>
-      <c r="C41" s="18">
+        <v>93</v>
+      </c>
+      <c r="C41" s="17">
         <v>16</v>
       </c>
-      <c r="D41" s="19">
+      <c r="D41" s="18">
         <v>527</v>
       </c>
       <c r="E41" s="7" t="s">
-        <v>7</v>
+        <v>22</v>
       </c>
       <c r="F41" s="10" t="s">
+        <v>282</v>
+      </c>
+      <c r="G41" s="12" t="s">
+        <v>281</v>
+      </c>
+      <c r="H41" s="26" t="s">
+        <v>280</v>
+      </c>
+      <c r="I41" s="21" t="s">
+        <v>279</v>
+      </c>
+      <c r="J41" s="21" t="s">
+        <v>278</v>
+      </c>
+      <c r="K41" s="21" t="s">
+        <v>277</v>
+      </c>
+      <c r="L41" s="12" t="s">
+        <v>276</v>
+      </c>
+      <c r="M41" s="13" t="s">
+        <v>275</v>
+      </c>
+      <c r="N41" s="27" t="s">
+        <v>274</v>
+      </c>
+      <c r="O41" s="10" t="s">
+        <v>273</v>
+      </c>
+      <c r="P41" s="10" t="s">
+        <v>272</v>
+      </c>
+      <c r="Q41" s="10" t="s">
+        <v>271</v>
+      </c>
+      <c r="R41" s="10" t="s">
+        <v>270</v>
+      </c>
+      <c r="S41" s="10" t="s">
+        <v>269</v>
+      </c>
+      <c r="T41" s="13" t="s">
+        <v>268</v>
+      </c>
+      <c r="U41" s="14" t="s">
         <v>267</v>
-      </c>
-      <c r="G41" s="12" t="s">
-        <v>266</v>
-      </c>
-      <c r="H41" s="27" t="s">
-        <v>265</v>
-      </c>
-      <c r="I41" s="22" t="s">
-        <v>264</v>
-      </c>
-      <c r="J41" s="22" t="s">
-        <v>263</v>
-      </c>
-      <c r="K41" s="22" t="s">
-        <v>262</v>
-      </c>
-      <c r="L41" s="12" t="s">
-        <v>261</v>
-      </c>
-      <c r="M41" s="13" t="s">
-        <v>260</v>
-      </c>
-      <c r="N41" s="28" t="s">
-        <v>259</v>
-      </c>
-      <c r="O41" s="10" t="s">
-        <v>258</v>
-      </c>
-      <c r="P41" s="10" t="s">
-        <v>257</v>
-      </c>
-      <c r="Q41" s="10" t="s">
-        <v>256</v>
-      </c>
-      <c r="R41" s="10" t="s">
-        <v>255</v>
-      </c>
-      <c r="S41" s="10" t="s">
-        <v>254</v>
-      </c>
-      <c r="T41" s="13" t="s">
-        <v>253</v>
-      </c>
-      <c r="U41" s="14" t="s">
-        <v>252</v>
       </c>
     </row>
     <row r="42" spans="2:21" ht="47.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B42" s="6" t="s">
-        <v>268</v>
-      </c>
-      <c r="C42" s="18">
+        <v>283</v>
+      </c>
+      <c r="C42" s="17">
         <v>8</v>
       </c>
-      <c r="D42" s="19">
+      <c r="D42" s="18">
         <v>529</v>
       </c>
       <c r="E42" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="F42" s="52"/>
-      <c r="G42" s="26"/>
-      <c r="H42" s="26"/>
-      <c r="I42" s="26"/>
-      <c r="J42" s="26"/>
-      <c r="K42" s="26"/>
-      <c r="L42" s="26"/>
-      <c r="M42" s="51"/>
-      <c r="N42" s="13" t="s">
-        <v>275</v>
-      </c>
-      <c r="O42" s="14" t="s">
-        <v>276</v>
-      </c>
-      <c r="P42" s="13" t="s">
-        <v>273</v>
-      </c>
-      <c r="Q42" s="14" t="s">
-        <v>274</v>
-      </c>
-      <c r="R42" s="13" t="s">
-        <v>271</v>
-      </c>
-      <c r="S42" s="14" t="s">
-        <v>272</v>
-      </c>
-      <c r="T42" s="13" t="s">
-        <v>270</v>
-      </c>
-      <c r="U42" s="14" t="s">
-        <v>269</v>
+        <v>22</v>
+      </c>
+      <c r="F42" s="53"/>
+      <c r="G42" s="25"/>
+      <c r="H42" s="25"/>
+      <c r="I42" s="25"/>
+      <c r="J42" s="25"/>
+      <c r="K42" s="25"/>
+      <c r="L42" s="25"/>
+      <c r="M42" s="52"/>
+      <c r="N42" s="21" t="s">
+        <v>290</v>
+      </c>
+      <c r="O42" s="21" t="s">
+        <v>291</v>
+      </c>
+      <c r="P42" s="21" t="s">
+        <v>288</v>
+      </c>
+      <c r="Q42" s="21" t="s">
+        <v>289</v>
+      </c>
+      <c r="R42" s="12" t="s">
+        <v>286</v>
+      </c>
+      <c r="S42" s="12" t="s">
+        <v>287</v>
+      </c>
+      <c r="T42" s="27" t="s">
+        <v>285</v>
+      </c>
+      <c r="U42" s="13" t="s">
+        <v>284</v>
       </c>
     </row>
     <row r="43" spans="2:21" ht="47.4" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B43" s="6" t="s">
-        <v>277</v>
-      </c>
-      <c r="C43" s="18">
+        <v>292</v>
+      </c>
+      <c r="C43" s="17">
         <v>8</v>
       </c>
-      <c r="D43" s="19">
+      <c r="D43" s="18">
         <v>530</v>
       </c>
       <c r="E43" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="F43" s="53"/>
-      <c r="G43" s="23"/>
-      <c r="H43" s="23"/>
-      <c r="I43" s="23"/>
-      <c r="J43" s="23"/>
-      <c r="K43" s="23"/>
-      <c r="L43" s="23"/>
-      <c r="M43" s="54"/>
-      <c r="N43" s="13" t="s">
-        <v>284</v>
-      </c>
-      <c r="O43" s="14" t="s">
-        <v>285</v>
-      </c>
-      <c r="P43" s="13" t="s">
-        <v>282</v>
-      </c>
-      <c r="Q43" s="14" t="s">
-        <v>283</v>
-      </c>
-      <c r="R43" s="13" t="s">
-        <v>280</v>
-      </c>
-      <c r="S43" s="14" t="s">
-        <v>281</v>
-      </c>
-      <c r="T43" s="13" t="s">
-        <v>279</v>
-      </c>
-      <c r="U43" s="14" t="s">
-        <v>278</v>
+        <v>22</v>
+      </c>
+      <c r="F43" s="54"/>
+      <c r="G43" s="22"/>
+      <c r="H43" s="22"/>
+      <c r="I43" s="22"/>
+      <c r="J43" s="22"/>
+      <c r="K43" s="22"/>
+      <c r="L43" s="22"/>
+      <c r="M43" s="55"/>
+      <c r="N43" s="21" t="s">
+        <v>299</v>
+      </c>
+      <c r="O43" s="21" t="s">
+        <v>300</v>
+      </c>
+      <c r="P43" s="21" t="s">
+        <v>297</v>
+      </c>
+      <c r="Q43" s="12" t="s">
+        <v>298</v>
+      </c>
+      <c r="R43" s="27" t="s">
+        <v>295</v>
+      </c>
+      <c r="S43" s="21" t="s">
+        <v>296</v>
+      </c>
+      <c r="T43" s="21" t="s">
+        <v>294</v>
+      </c>
+      <c r="U43" s="13" t="s">
+        <v>293</v>
       </c>
     </row>
     <row r="44" spans="2:21" ht="63" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B44" s="6" t="s">
-        <v>286</v>
-      </c>
-      <c r="C44" s="18">
+        <v>301</v>
+      </c>
+      <c r="C44" s="17">
         <v>8</v>
       </c>
-      <c r="D44" s="19">
+      <c r="D44" s="18">
         <v>531</v>
       </c>
       <c r="E44" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="F44" s="53"/>
-      <c r="G44" s="23"/>
-      <c r="H44" s="23"/>
-      <c r="I44" s="23"/>
-      <c r="J44" s="23"/>
-      <c r="K44" s="23"/>
-      <c r="L44" s="23"/>
-      <c r="M44" s="54"/>
-      <c r="N44" s="14" t="s">
-        <v>293</v>
-      </c>
-      <c r="O44" s="14" t="s">
-        <v>294</v>
-      </c>
-      <c r="P44" s="14" t="s">
-        <v>291</v>
-      </c>
-      <c r="Q44" s="14" t="s">
-        <v>292</v>
-      </c>
-      <c r="R44" s="14" t="s">
-        <v>289</v>
-      </c>
-      <c r="S44" s="14" t="s">
-        <v>290</v>
-      </c>
-      <c r="T44" s="14" t="s">
-        <v>288</v>
-      </c>
-      <c r="U44" s="14" t="s">
-        <v>287</v>
+        <v>22</v>
+      </c>
+      <c r="F44" s="54"/>
+      <c r="G44" s="22"/>
+      <c r="H44" s="22"/>
+      <c r="I44" s="22"/>
+      <c r="J44" s="22"/>
+      <c r="K44" s="22"/>
+      <c r="L44" s="22"/>
+      <c r="M44" s="55"/>
+      <c r="N44" s="10" t="s">
+        <v>308</v>
+      </c>
+      <c r="O44" s="12" t="s">
+        <v>309</v>
+      </c>
+      <c r="P44" s="12" t="s">
+        <v>306</v>
+      </c>
+      <c r="Q44" s="12" t="s">
+        <v>307</v>
+      </c>
+      <c r="R44" s="12" t="s">
+        <v>304</v>
+      </c>
+      <c r="S44" s="26" t="s">
+        <v>305</v>
+      </c>
+      <c r="T44" s="12" t="s">
+        <v>303</v>
+      </c>
+      <c r="U44" s="13" t="s">
+        <v>302</v>
       </c>
     </row>
     <row r="45" spans="2:21" ht="63" thickBot="1" x14ac:dyDescent="0.35">
       <c r="B45" s="6" t="s">
-        <v>295</v>
-      </c>
-      <c r="C45" s="18">
+        <v>310</v>
+      </c>
+      <c r="C45" s="17">
         <v>8</v>
       </c>
-      <c r="D45" s="19">
+      <c r="D45" s="18">
         <v>532</v>
       </c>
       <c r="E45" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="F45" s="56"/>
+      <c r="G45" s="26"/>
+      <c r="H45" s="26"/>
+      <c r="I45" s="26"/>
+      <c r="J45" s="26"/>
+      <c r="K45" s="26"/>
+      <c r="L45" s="26"/>
+      <c r="M45" s="51"/>
+      <c r="N45" s="10" t="s">
+        <v>318</v>
+      </c>
+      <c r="O45" s="21" t="s">
+        <v>317</v>
+      </c>
+      <c r="P45" s="21" t="s">
+        <v>315</v>
+      </c>
+      <c r="Q45" s="21" t="s">
+        <v>316</v>
+      </c>
+      <c r="R45" s="12" t="s">
+        <v>313</v>
+      </c>
+      <c r="S45" s="26" t="s">
+        <v>314</v>
+      </c>
+      <c r="T45" s="12" t="s">
+        <v>312</v>
+      </c>
+      <c r="U45" s="51" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="46" spans="2:21" ht="47.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B46" s="6" t="s">
+        <v>319</v>
+      </c>
+      <c r="C46" s="17">
+        <v>16</v>
+      </c>
+      <c r="D46" s="18">
+        <v>533</v>
+      </c>
+      <c r="E46" s="7" t="s">
+        <v>333</v>
+      </c>
+      <c r="F46" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="G46" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="H46" s="26" t="s">
+        <v>332</v>
+      </c>
+      <c r="I46" s="10" t="s">
+        <v>331</v>
+      </c>
+      <c r="J46" s="12" t="s">
+        <v>330</v>
+      </c>
+      <c r="K46" s="10" t="s">
+        <v>329</v>
+      </c>
+      <c r="L46" s="10" t="s">
+        <v>328</v>
+      </c>
+      <c r="M46" s="21" t="s">
+        <v>327</v>
+      </c>
+      <c r="N46" s="11" t="s">
+        <v>326</v>
+      </c>
+      <c r="O46" s="10" t="s">
+        <v>325</v>
+      </c>
+      <c r="P46" s="10" t="s">
+        <v>324</v>
+      </c>
+      <c r="Q46" s="10" t="s">
+        <v>323</v>
+      </c>
+      <c r="R46" s="10" t="s">
+        <v>322</v>
+      </c>
+      <c r="S46" s="10" t="s">
+        <v>321</v>
+      </c>
+      <c r="T46" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="U46" s="51" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="47" spans="2:21" ht="47.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B47" s="6" t="s">
+        <v>334</v>
+      </c>
+      <c r="C47" s="17">
+        <v>16</v>
+      </c>
+      <c r="D47" s="18">
+        <v>535</v>
+      </c>
+      <c r="E47" s="7" t="s">
+        <v>333</v>
+      </c>
+      <c r="F47" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="G47" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="H47" s="26" t="s">
+        <v>332</v>
+      </c>
+      <c r="I47" s="10" t="s">
+        <v>331</v>
+      </c>
+      <c r="J47" s="12" t="s">
+        <v>330</v>
+      </c>
+      <c r="K47" s="10" t="s">
+        <v>329</v>
+      </c>
+      <c r="L47" s="10" t="s">
+        <v>328</v>
+      </c>
+      <c r="M47" s="21" t="s">
+        <v>327</v>
+      </c>
+      <c r="N47" s="11" t="s">
+        <v>326</v>
+      </c>
+      <c r="O47" s="10" t="s">
+        <v>325</v>
+      </c>
+      <c r="P47" s="10" t="s">
+        <v>324</v>
+      </c>
+      <c r="Q47" s="10" t="s">
+        <v>323</v>
+      </c>
+      <c r="R47" s="10" t="s">
+        <v>322</v>
+      </c>
+      <c r="S47" s="10" t="s">
+        <v>321</v>
+      </c>
+      <c r="T47" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="U47" s="51" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="48" spans="2:21" ht="47.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B48" s="6" t="s">
+        <v>335</v>
+      </c>
+      <c r="C48" s="17">
+        <v>16</v>
+      </c>
+      <c r="D48" s="18">
+        <v>537</v>
+      </c>
+      <c r="E48" s="7" t="s">
+        <v>333</v>
+      </c>
+      <c r="F48" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="G48" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="H48" s="26" t="s">
+        <v>332</v>
+      </c>
+      <c r="I48" s="10" t="s">
+        <v>331</v>
+      </c>
+      <c r="J48" s="12" t="s">
+        <v>330</v>
+      </c>
+      <c r="K48" s="10" t="s">
+        <v>329</v>
+      </c>
+      <c r="L48" s="10" t="s">
+        <v>328</v>
+      </c>
+      <c r="M48" s="21" t="s">
+        <v>327</v>
+      </c>
+      <c r="N48" s="11" t="s">
+        <v>326</v>
+      </c>
+      <c r="O48" s="10" t="s">
+        <v>325</v>
+      </c>
+      <c r="P48" s="10" t="s">
+        <v>324</v>
+      </c>
+      <c r="Q48" s="10" t="s">
+        <v>323</v>
+      </c>
+      <c r="R48" s="10" t="s">
+        <v>322</v>
+      </c>
+      <c r="S48" s="10" t="s">
+        <v>321</v>
+      </c>
+      <c r="T48" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="U48" s="51" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="49" spans="1:21" ht="47.4" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B49" s="6" t="s">
+        <v>336</v>
+      </c>
+      <c r="C49" s="17">
+        <v>16</v>
+      </c>
+      <c r="D49" s="18">
+        <v>539</v>
+      </c>
+      <c r="E49" s="7" t="s">
+        <v>333</v>
+      </c>
+      <c r="F49" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="G49" s="18" t="s">
+        <v>34</v>
+      </c>
+      <c r="H49" s="26" t="s">
+        <v>332</v>
+      </c>
+      <c r="I49" s="10" t="s">
+        <v>331</v>
+      </c>
+      <c r="J49" s="12" t="s">
+        <v>330</v>
+      </c>
+      <c r="K49" s="10" t="s">
+        <v>329</v>
+      </c>
+      <c r="L49" s="10" t="s">
+        <v>328</v>
+      </c>
+      <c r="M49" s="21" t="s">
+        <v>327</v>
+      </c>
+      <c r="N49" s="11" t="s">
+        <v>326</v>
+      </c>
+      <c r="O49" s="10" t="s">
+        <v>325</v>
+      </c>
+      <c r="P49" s="10" t="s">
+        <v>324</v>
+      </c>
+      <c r="Q49" s="10" t="s">
+        <v>323</v>
+      </c>
+      <c r="R49" s="10" t="s">
+        <v>322</v>
+      </c>
+      <c r="S49" s="10" t="s">
+        <v>321</v>
+      </c>
+      <c r="T49" s="12" t="s">
+        <v>120</v>
+      </c>
+      <c r="U49" s="51" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="50" spans="1:21" ht="34.200000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B50" s="6" t="s">
+        <v>337</v>
+      </c>
+      <c r="C50" s="17">
+        <v>16</v>
+      </c>
+      <c r="D50" s="18">
+        <v>541</v>
+      </c>
+      <c r="E50" s="7" t="s">
+        <v>333</v>
+      </c>
+      <c r="F50" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="G50" s="18" t="s">
+        <v>352</v>
+      </c>
+      <c r="H50" s="26" t="s">
+        <v>351</v>
+      </c>
+      <c r="I50" s="10" t="s">
+        <v>350</v>
+      </c>
+      <c r="J50" s="12" t="s">
+        <v>349</v>
+      </c>
+      <c r="K50" s="10" t="s">
+        <v>348</v>
+      </c>
+      <c r="L50" s="10" t="s">
+        <v>347</v>
+      </c>
+      <c r="M50" s="21" t="s">
+        <v>346</v>
+      </c>
+      <c r="N50" s="11" t="s">
+        <v>345</v>
+      </c>
+      <c r="O50" s="10" t="s">
+        <v>344</v>
+      </c>
+      <c r="P50" s="10" t="s">
+        <v>343</v>
+      </c>
+      <c r="Q50" s="10" t="s">
+        <v>342</v>
+      </c>
+      <c r="R50" s="10" t="s">
+        <v>341</v>
+      </c>
+      <c r="S50" s="10" t="s">
+        <v>340</v>
+      </c>
+      <c r="T50" s="12" t="s">
+        <v>339</v>
+      </c>
+      <c r="U50" s="51" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="51" spans="1:21" ht="36" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B51" s="6" t="s">
+        <v>353</v>
+      </c>
+      <c r="C51" s="17">
+        <v>16</v>
+      </c>
+      <c r="D51" s="18">
+        <v>543</v>
+      </c>
+      <c r="E51" s="7" t="s">
+        <v>333</v>
+      </c>
+      <c r="F51" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="G51" s="18" t="s">
+        <v>352</v>
+      </c>
+      <c r="H51" s="26" t="s">
+        <v>351</v>
+      </c>
+      <c r="I51" s="10" t="s">
+        <v>350</v>
+      </c>
+      <c r="J51" s="12" t="s">
+        <v>349</v>
+      </c>
+      <c r="K51" s="10" t="s">
+        <v>348</v>
+      </c>
+      <c r="L51" s="10" t="s">
+        <v>347</v>
+      </c>
+      <c r="M51" s="21" t="s">
+        <v>346</v>
+      </c>
+      <c r="N51" s="11" t="s">
+        <v>345</v>
+      </c>
+      <c r="O51" s="10" t="s">
+        <v>344</v>
+      </c>
+      <c r="P51" s="10" t="s">
+        <v>343</v>
+      </c>
+      <c r="Q51" s="10" t="s">
+        <v>342</v>
+      </c>
+      <c r="R51" s="10" t="s">
+        <v>341</v>
+      </c>
+      <c r="S51" s="10" t="s">
+        <v>340</v>
+      </c>
+      <c r="T51" s="12" t="s">
+        <v>339</v>
+      </c>
+      <c r="U51" s="51" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="52" spans="1:21" ht="34.200000000000003" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B52" s="6" t="s">
+        <v>354</v>
+      </c>
+      <c r="C52" s="17">
+        <v>16</v>
+      </c>
+      <c r="D52" s="18">
+        <v>545</v>
+      </c>
+      <c r="E52" s="7" t="s">
+        <v>333</v>
+      </c>
+      <c r="F52" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="G52" s="18" t="s">
+        <v>352</v>
+      </c>
+      <c r="H52" s="26" t="s">
+        <v>351</v>
+      </c>
+      <c r="I52" s="10" t="s">
+        <v>350</v>
+      </c>
+      <c r="J52" s="12" t="s">
+        <v>349</v>
+      </c>
+      <c r="K52" s="10" t="s">
+        <v>348</v>
+      </c>
+      <c r="L52" s="10" t="s">
+        <v>347</v>
+      </c>
+      <c r="M52" s="21" t="s">
+        <v>346</v>
+      </c>
+      <c r="N52" s="11" t="s">
+        <v>345</v>
+      </c>
+      <c r="O52" s="10" t="s">
+        <v>344</v>
+      </c>
+      <c r="P52" s="10" t="s">
+        <v>343</v>
+      </c>
+      <c r="Q52" s="10" t="s">
+        <v>342</v>
+      </c>
+      <c r="R52" s="10" t="s">
+        <v>341</v>
+      </c>
+      <c r="S52" s="10" t="s">
+        <v>340</v>
+      </c>
+      <c r="T52" s="12" t="s">
+        <v>339</v>
+      </c>
+      <c r="U52" s="51" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="53" spans="1:21" ht="33.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B53" s="6" t="s">
+        <v>356</v>
+      </c>
+      <c r="C53" s="17">
+        <v>16</v>
+      </c>
+      <c r="D53" s="18">
+        <v>547</v>
+      </c>
+      <c r="E53" s="7" t="s">
+        <v>333</v>
+      </c>
+      <c r="F53" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="G53" s="18" t="s">
+        <v>352</v>
+      </c>
+      <c r="H53" s="26" t="s">
+        <v>351</v>
+      </c>
+      <c r="I53" s="10" t="s">
+        <v>350</v>
+      </c>
+      <c r="J53" s="12" t="s">
+        <v>349</v>
+      </c>
+      <c r="K53" s="10" t="s">
+        <v>348</v>
+      </c>
+      <c r="L53" s="10" t="s">
+        <v>347</v>
+      </c>
+      <c r="M53" s="21" t="s">
+        <v>346</v>
+      </c>
+      <c r="N53" s="11" t="s">
+        <v>345</v>
+      </c>
+      <c r="O53" s="10" t="s">
+        <v>344</v>
+      </c>
+      <c r="P53" s="10" t="s">
+        <v>343</v>
+      </c>
+      <c r="Q53" s="10" t="s">
+        <v>342</v>
+      </c>
+      <c r="R53" s="10" t="s">
+        <v>341</v>
+      </c>
+      <c r="S53" s="10" t="s">
+        <v>340</v>
+      </c>
+      <c r="T53" s="12" t="s">
+        <v>339</v>
+      </c>
+      <c r="U53" s="51" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="54" spans="1:21" ht="33" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B54" s="6" t="s">
+        <v>355</v>
+      </c>
+      <c r="C54" s="17">
+        <v>16</v>
+      </c>
+      <c r="D54" s="18">
+        <v>549</v>
+      </c>
+      <c r="E54" s="7" t="s">
+        <v>333</v>
+      </c>
+      <c r="F54" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="G54" s="18" t="s">
+        <v>352</v>
+      </c>
+      <c r="H54" s="26" t="s">
+        <v>351</v>
+      </c>
+      <c r="I54" s="10" t="s">
+        <v>350</v>
+      </c>
+      <c r="J54" s="12" t="s">
+        <v>349</v>
+      </c>
+      <c r="K54" s="10" t="s">
+        <v>348</v>
+      </c>
+      <c r="L54" s="10" t="s">
+        <v>347</v>
+      </c>
+      <c r="M54" s="21" t="s">
+        <v>346</v>
+      </c>
+      <c r="N54" s="11" t="s">
+        <v>345</v>
+      </c>
+      <c r="O54" s="10" t="s">
+        <v>344</v>
+      </c>
+      <c r="P54" s="10" t="s">
+        <v>343</v>
+      </c>
+      <c r="Q54" s="10" t="s">
+        <v>342</v>
+      </c>
+      <c r="R54" s="10" t="s">
+        <v>341</v>
+      </c>
+      <c r="S54" s="10" t="s">
+        <v>340</v>
+      </c>
+      <c r="T54" s="12" t="s">
+        <v>339</v>
+      </c>
+      <c r="U54" s="51" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="55" spans="1:21" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B55" s="6" t="s">
+        <v>357</v>
+      </c>
+      <c r="C55" s="17">
+        <v>16</v>
+      </c>
+      <c r="D55" s="18">
+        <v>551</v>
+      </c>
+      <c r="E55" s="7" t="s">
+        <v>333</v>
+      </c>
+      <c r="F55" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="G55" s="18" t="s">
+        <v>352</v>
+      </c>
+      <c r="H55" s="26" t="s">
+        <v>351</v>
+      </c>
+      <c r="I55" s="10" t="s">
+        <v>350</v>
+      </c>
+      <c r="J55" s="12" t="s">
+        <v>349</v>
+      </c>
+      <c r="K55" s="10" t="s">
+        <v>348</v>
+      </c>
+      <c r="L55" s="10" t="s">
+        <v>347</v>
+      </c>
+      <c r="M55" s="21" t="s">
+        <v>346</v>
+      </c>
+      <c r="N55" s="11" t="s">
+        <v>345</v>
+      </c>
+      <c r="O55" s="10" t="s">
+        <v>344</v>
+      </c>
+      <c r="P55" s="10" t="s">
+        <v>343</v>
+      </c>
+      <c r="Q55" s="10" t="s">
+        <v>342</v>
+      </c>
+      <c r="R55" s="10" t="s">
+        <v>341</v>
+      </c>
+      <c r="S55" s="10" t="s">
+        <v>340</v>
+      </c>
+      <c r="T55" s="12" t="s">
+        <v>339</v>
+      </c>
+      <c r="U55" s="51" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="56" spans="1:21" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B56" s="6" t="s">
+        <v>358</v>
+      </c>
+      <c r="C56" s="17">
+        <v>16</v>
+      </c>
+      <c r="D56" s="18">
+        <v>553</v>
+      </c>
+      <c r="E56" s="7" t="s">
+        <v>333</v>
+      </c>
+      <c r="F56" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="G56" s="18" t="s">
+        <v>352</v>
+      </c>
+      <c r="H56" s="26" t="s">
+        <v>351</v>
+      </c>
+      <c r="I56" s="10" t="s">
+        <v>350</v>
+      </c>
+      <c r="J56" s="12" t="s">
+        <v>349</v>
+      </c>
+      <c r="K56" s="10" t="s">
+        <v>348</v>
+      </c>
+      <c r="L56" s="10" t="s">
+        <v>347</v>
+      </c>
+      <c r="M56" s="21" t="s">
+        <v>346</v>
+      </c>
+      <c r="N56" s="11" t="s">
+        <v>345</v>
+      </c>
+      <c r="O56" s="10" t="s">
+        <v>344</v>
+      </c>
+      <c r="P56" s="10" t="s">
+        <v>343</v>
+      </c>
+      <c r="Q56" s="10" t="s">
+        <v>342</v>
+      </c>
+      <c r="R56" s="10" t="s">
+        <v>341</v>
+      </c>
+      <c r="S56" s="10" t="s">
+        <v>340</v>
+      </c>
+      <c r="T56" s="12" t="s">
+        <v>339</v>
+      </c>
+      <c r="U56" s="51" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="57" spans="1:21" ht="30.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B57" s="6" t="s">
+        <v>359</v>
+      </c>
+      <c r="C57" s="17">
+        <v>16</v>
+      </c>
+      <c r="D57" s="18">
+        <v>555</v>
+      </c>
+      <c r="E57" s="7" t="s">
+        <v>333</v>
+      </c>
+      <c r="F57" s="17" t="s">
+        <v>34</v>
+      </c>
+      <c r="G57" s="18" t="s">
+        <v>352</v>
+      </c>
+      <c r="H57" s="26" t="s">
+        <v>351</v>
+      </c>
+      <c r="I57" s="10" t="s">
+        <v>350</v>
+      </c>
+      <c r="J57" s="12" t="s">
+        <v>349</v>
+      </c>
+      <c r="K57" s="10" t="s">
+        <v>348</v>
+      </c>
+      <c r="L57" s="10" t="s">
+        <v>347</v>
+      </c>
+      <c r="M57" s="21" t="s">
+        <v>346</v>
+      </c>
+      <c r="N57" s="11" t="s">
+        <v>345</v>
+      </c>
+      <c r="O57" s="10" t="s">
+        <v>344</v>
+      </c>
+      <c r="P57" s="10" t="s">
+        <v>343</v>
+      </c>
+      <c r="Q57" s="10" t="s">
+        <v>342</v>
+      </c>
+      <c r="R57" s="10" t="s">
+        <v>341</v>
+      </c>
+      <c r="S57" s="10" t="s">
+        <v>340</v>
+      </c>
+      <c r="T57" s="12" t="s">
+        <v>339</v>
+      </c>
+      <c r="U57" s="51" t="s">
+        <v>338</v>
+      </c>
+    </row>
+    <row r="58" spans="1:21" ht="30.6" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="B58" s="22"/>
+      <c r="C58" s="23"/>
+      <c r="D58" s="23"/>
+      <c r="E58" s="24"/>
+      <c r="F58" s="23"/>
+      <c r="G58" s="23"/>
+      <c r="H58" s="22"/>
+      <c r="I58" s="22"/>
+      <c r="J58" s="22"/>
+      <c r="K58" s="22"/>
+      <c r="L58" s="22"/>
+      <c r="M58" s="22"/>
+      <c r="N58" s="22"/>
+      <c r="O58" s="22"/>
+      <c r="P58" s="22"/>
+      <c r="Q58" s="22"/>
+      <c r="R58" s="22"/>
+      <c r="S58" s="22"/>
+      <c r="T58" s="22"/>
+      <c r="U58" s="22"/>
+    </row>
+    <row r="59" spans="1:21" ht="30.6" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B59" s="22"/>
+      <c r="C59" s="23"/>
+      <c r="D59" s="23"/>
+      <c r="E59" s="24"/>
+      <c r="F59" s="23"/>
+      <c r="G59" s="23"/>
+      <c r="H59" s="22"/>
+      <c r="I59" s="22"/>
+      <c r="J59" s="22"/>
+      <c r="K59" s="22"/>
+      <c r="L59" s="22"/>
+      <c r="M59" s="22"/>
+      <c r="N59" s="22"/>
+      <c r="O59" s="22"/>
+      <c r="P59" s="22"/>
+      <c r="Q59" s="22"/>
+      <c r="R59" s="22"/>
+      <c r="S59" s="22"/>
+      <c r="T59" s="22"/>
+      <c r="U59" s="22"/>
+    </row>
+    <row r="60" spans="1:21" ht="44.4" customHeight="1" thickBot="1" x14ac:dyDescent="0.9">
+      <c r="A60" s="57"/>
+      <c r="B60" s="58" t="s">
+        <v>360</v>
+      </c>
+      <c r="C60" s="59"/>
+      <c r="D60" s="59"/>
+      <c r="E60" s="59"/>
+      <c r="F60" s="59"/>
+      <c r="G60" s="59"/>
+      <c r="H60" s="59"/>
+      <c r="I60" s="59"/>
+      <c r="J60" s="59"/>
+      <c r="K60" s="59"/>
+      <c r="L60" s="59"/>
+      <c r="M60" s="60"/>
+    </row>
+    <row r="61" spans="1:21" ht="16.2" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B61" s="35" t="s">
+        <v>3</v>
+      </c>
+      <c r="C61" s="37" t="s">
+        <v>2</v>
+      </c>
+      <c r="D61" s="39" t="s">
+        <v>1</v>
+      </c>
+      <c r="E61" s="41" t="s">
+        <v>0</v>
+      </c>
+      <c r="F61" s="43" t="s">
+        <v>4</v>
+      </c>
+      <c r="G61" s="44"/>
+      <c r="H61" s="44"/>
+      <c r="I61" s="44"/>
+      <c r="J61" s="44"/>
+      <c r="K61" s="44"/>
+      <c r="L61" s="44"/>
+      <c r="M61" s="48"/>
+    </row>
+    <row r="62" spans="1:21" ht="93" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B62" s="36"/>
+      <c r="C62" s="38"/>
+      <c r="D62" s="40"/>
+      <c r="E62" s="42"/>
+      <c r="F62" s="30">
         <v>7</v>
       </c>
-      <c r="F45" s="55"/>
-      <c r="G45" s="27"/>
-      <c r="H45" s="27"/>
-      <c r="I45" s="23"/>
-      <c r="J45" s="23"/>
-      <c r="K45" s="23"/>
-      <c r="L45" s="23"/>
-      <c r="M45" s="54"/>
-      <c r="N45" s="14" t="s">
-        <v>303</v>
-      </c>
-      <c r="O45" s="14" t="s">
-        <v>302</v>
-      </c>
-      <c r="P45" s="14" t="s">
-        <v>300</v>
-      </c>
-      <c r="Q45" s="14" t="s">
-        <v>301</v>
-      </c>
-      <c r="R45" s="14" t="s">
-        <v>298</v>
-      </c>
-      <c r="S45" s="14" t="s">
-        <v>299</v>
-      </c>
-      <c r="T45" s="14" t="s">
-        <v>297</v>
-      </c>
-      <c r="U45" s="14" t="s">
-        <v>296</v>
-      </c>
-    </row>
-    <row r="46" spans="2:21" ht="31.8" thickBot="1" x14ac:dyDescent="0.35">
-      <c r="B46" s="6"/>
-      <c r="C46" s="18">
+      <c r="G62" s="31">
+        <v>6</v>
+      </c>
+      <c r="H62" s="31">
+        <v>5</v>
+      </c>
+      <c r="I62" s="32">
+        <v>4</v>
+      </c>
+      <c r="J62" s="15">
+        <v>3</v>
+      </c>
+      <c r="K62" s="31">
+        <v>2</v>
+      </c>
+      <c r="L62" s="31">
+        <v>1</v>
+      </c>
+      <c r="M62" s="32">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="63" spans="1:21" ht="84" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B63" s="6" t="s">
+        <v>361</v>
+      </c>
+      <c r="C63" s="17">
+        <v>8</v>
+      </c>
+      <c r="D63" s="18">
+        <v>88</v>
+      </c>
+      <c r="E63" s="7" t="s">
+        <v>333</v>
+      </c>
+      <c r="F63" s="11" t="s">
+        <v>371</v>
+      </c>
+      <c r="G63" s="12" t="s">
+        <v>370</v>
+      </c>
+      <c r="H63" s="12" t="s">
+        <v>369</v>
+      </c>
+      <c r="I63" s="28" t="s">
+        <v>368</v>
+      </c>
+      <c r="J63" s="11" t="s">
+        <v>367</v>
+      </c>
+      <c r="K63" s="27" t="s">
+        <v>366</v>
+      </c>
+      <c r="L63" s="12" t="s">
+        <v>365</v>
+      </c>
+      <c r="M63" s="28" t="s">
+        <v>364</v>
+      </c>
+    </row>
+    <row r="64" spans="1:21" ht="84" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B64" s="6" t="s">
+        <v>362</v>
+      </c>
+      <c r="C64" s="17">
+        <v>8</v>
+      </c>
+      <c r="D64" s="18">
+        <v>89</v>
+      </c>
+      <c r="E64" s="7" t="s">
+        <v>333</v>
+      </c>
+      <c r="F64" s="21" t="s">
+        <v>379</v>
+      </c>
+      <c r="G64" s="12" t="s">
+        <v>378</v>
+      </c>
+      <c r="H64" s="27" t="s">
+        <v>376</v>
+      </c>
+      <c r="I64" s="13" t="s">
+        <v>377</v>
+      </c>
+      <c r="J64" s="21" t="s">
+        <v>375</v>
+      </c>
+      <c r="K64" s="12" t="s">
+        <v>374</v>
+      </c>
+      <c r="L64" s="27" t="s">
+        <v>373</v>
+      </c>
+      <c r="M64" s="13" t="s">
+        <v>372</v>
+      </c>
+    </row>
+    <row r="65" spans="2:13" ht="84" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B65" s="6" t="s">
+        <v>363</v>
+      </c>
+      <c r="C65" s="17">
+        <v>8</v>
+      </c>
+      <c r="D65" s="18">
+        <v>90</v>
+      </c>
+      <c r="E65" s="7" t="s">
+        <v>333</v>
+      </c>
+      <c r="F65" s="11" t="s">
+        <v>384</v>
+      </c>
+      <c r="G65" s="27" t="s">
+        <v>387</v>
+      </c>
+      <c r="H65" s="12" t="s">
+        <v>386</v>
+      </c>
+      <c r="I65" s="28" t="s">
+        <v>385</v>
+      </c>
+      <c r="J65" s="11" t="s">
+        <v>383</v>
+      </c>
+      <c r="K65" s="16" t="s">
+        <v>382</v>
+      </c>
+      <c r="L65" s="16" t="s">
+        <v>381</v>
+      </c>
+      <c r="M65" s="28" t="s">
+        <v>380</v>
+      </c>
+    </row>
+    <row r="66" spans="2:13" ht="84" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B66" s="6" t="s">
+        <v>388</v>
+      </c>
+      <c r="C66" s="17">
+        <v>8</v>
+      </c>
+      <c r="D66" s="18">
+        <v>91</v>
+      </c>
+      <c r="E66" s="7" t="s">
+        <v>333</v>
+      </c>
+      <c r="F66" s="11" t="s">
+        <v>11</v>
+      </c>
+      <c r="G66" s="27" t="s">
+        <v>10</v>
+      </c>
+      <c r="H66" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="I66" s="28" t="s">
+        <v>8</v>
+      </c>
+      <c r="J66" s="11" t="s">
+        <v>7</v>
+      </c>
+      <c r="K66" s="16" t="s">
+        <v>6</v>
+      </c>
+      <c r="L66" s="16" t="s">
+        <v>5</v>
+      </c>
+      <c r="M66" s="28" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="67" spans="2:13" ht="84" customHeight="1" thickBot="1" x14ac:dyDescent="0.35">
+      <c r="B67" s="6" t="s">
+        <v>389</v>
+      </c>
+      <c r="C67" s="17">
+        <v>8</v>
+      </c>
+      <c r="D67" s="18">
+        <v>92</v>
+      </c>
+      <c r="E67" s="7" t="s">
+        <v>333</v>
+      </c>
+      <c r="F67" s="11" t="s">
+        <v>19</v>
+      </c>
+      <c r="G67" s="27" t="s">
+        <v>18</v>
+      </c>
+      <c r="H67" s="12" t="s">
+        <v>17</v>
+      </c>
+      <c r="I67" s="28" t="s">
+        <v>390</v>
+      </c>
+      <c r="J67" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="D46" s="19"/>
-      <c r="E46" s="7" t="s">
-        <v>7</v>
-      </c>
-      <c r="F46" s="10"/>
-      <c r="G46" s="9"/>
-      <c r="H46" s="27"/>
-      <c r="I46" s="22"/>
-      <c r="J46" s="22"/>
-      <c r="K46" s="22"/>
-      <c r="L46" s="12"/>
-      <c r="M46" s="13"/>
-      <c r="N46" s="28"/>
-      <c r="O46" s="10"/>
-      <c r="P46" s="10"/>
-      <c r="Q46" s="10"/>
-      <c r="R46" s="10"/>
-      <c r="S46" s="10"/>
-      <c r="T46" s="13"/>
-      <c r="U46" s="14"/>
-    </row>
-    <row r="47" spans="2:21" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="N47" s="15"/>
-      <c r="O47" s="15"/>
-      <c r="P47" s="15"/>
-      <c r="Q47" s="15"/>
-      <c r="R47" s="15"/>
-      <c r="S47" s="15"/>
-      <c r="T47" s="15"/>
-      <c r="U47" s="15"/>
-    </row>
-    <row r="48" spans="2:21" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="N48" s="15"/>
-      <c r="O48" s="15"/>
-      <c r="P48" s="15"/>
-      <c r="Q48" s="15"/>
-      <c r="R48" s="15"/>
-      <c r="S48" s="15"/>
-      <c r="T48" s="15"/>
-      <c r="U48" s="15"/>
-    </row>
-    <row r="50" spans="14:21" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="N50" s="21"/>
-      <c r="O50" s="21"/>
-      <c r="P50" s="21"/>
-      <c r="Q50" s="21"/>
-      <c r="R50" s="21"/>
-      <c r="S50" s="21"/>
-      <c r="T50" s="21"/>
-      <c r="U50" s="21"/>
-    </row>
-    <row r="52" spans="14:21" ht="93" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="53" spans="14:21" ht="27" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="54" spans="14:21" ht="33" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="55" spans="14:21" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="N55" s="21"/>
-      <c r="O55" s="21"/>
-      <c r="P55" s="21"/>
-      <c r="Q55" s="21"/>
-      <c r="R55" s="21"/>
-      <c r="S55" s="21"/>
-      <c r="T55" s="21"/>
-      <c r="U55" s="21"/>
-    </row>
-    <row r="57" spans="14:21" ht="93" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="58" spans="14:21" ht="84" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="59" spans="14:21" ht="84" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="60" spans="14:21" ht="84" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="63" spans="14:21" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="N63" s="21"/>
-      <c r="O63" s="21"/>
-      <c r="P63" s="21"/>
-      <c r="Q63" s="21"/>
-      <c r="R63" s="21"/>
-      <c r="S63" s="21"/>
-      <c r="T63" s="21"/>
-      <c r="U63" s="21"/>
-    </row>
-    <row r="65" ht="93" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="66" ht="84" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="67" ht="84" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="68" ht="84" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="69" ht="84" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="70" ht="84" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="71" ht="84" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="72" ht="84" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="73" ht="84" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="74" ht="84" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="75" ht="84" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="76" ht="84" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="77" ht="84" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="78" ht="84" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="79" ht="84" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="80" ht="84" customHeight="1" x14ac:dyDescent="0.3"/>
+      <c r="K67" s="16" t="s">
+        <v>15</v>
+      </c>
+      <c r="L67" s="16" t="s">
+        <v>14</v>
+      </c>
+      <c r="M67" s="28" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="68" spans="2:13" ht="84" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="69" spans="2:13" ht="84" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="70" spans="2:13" ht="84" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="71" spans="2:13" ht="84" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="72" spans="2:13" ht="84" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="73" spans="2:13" ht="84" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="74" spans="2:13" ht="84" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="75" spans="2:13" ht="84" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="76" spans="2:13" ht="84" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="77" spans="2:13" ht="84" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="78" spans="2:13" ht="84" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="79" spans="2:13" ht="84" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="80" spans="2:13" ht="84" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="81" ht="84" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="82" ht="84" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="83" ht="84" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -3942,28 +5199,28 @@
     <row r="94" ht="84" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="95" ht="84" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="96" ht="84" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="97" ht="84" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="98" ht="84" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="99" ht="84" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="100" ht="84" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="101" ht="84" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="102" ht="84" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="103" ht="84" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="104" ht="84" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="105" ht="84" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="106" ht="84" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="107" ht="84" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="108" ht="84" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="109" ht="84" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="110" ht="84" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="111" ht="84" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="112" ht="84" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="97" spans="18:18" ht="84" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="98" spans="18:18" ht="84" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="99" spans="18:18" ht="84" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="100" spans="18:18" ht="84" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="101" spans="18:18" ht="84" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="102" spans="18:18" ht="84" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="103" spans="18:18" ht="84" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="104" spans="18:18" ht="84" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="105" spans="18:18" ht="84" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="106" spans="18:18" ht="84" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="107" spans="18:18" ht="84" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="108" spans="18:18" ht="84" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="109" spans="18:18" ht="84" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="110" spans="18:18" ht="84" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="111" spans="18:18" ht="84" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="R111" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="112" spans="18:18" ht="84" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="113" spans="14:21" ht="84" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="114" spans="14:21" ht="84" customHeight="1" x14ac:dyDescent="0.3">
-      <c r="R114" t="s">
-        <v>5</v>
-      </c>
-    </row>
+    <row r="114" spans="14:21" ht="84" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="115" spans="14:21" ht="84" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="116" spans="14:21" ht="84" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="117" spans="14:21" ht="84" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -3971,19 +5228,19 @@
     <row r="119" spans="14:21" ht="84" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="120" spans="14:21" ht="84" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="121" spans="14:21" ht="84" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="122" spans="14:21" ht="84" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="123" spans="14:21" ht="84" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="124" spans="14:21" ht="84" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="127" spans="14:21" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="N127" s="21"/>
-      <c r="O127" s="21"/>
-      <c r="P127" s="21"/>
-      <c r="Q127" s="21"/>
-      <c r="R127" s="21"/>
-      <c r="S127" s="21"/>
-      <c r="T127" s="21"/>
-      <c r="U127" s="21"/>
-    </row>
+    <row r="124" spans="14:21" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="N124" s="20"/>
+      <c r="O124" s="20"/>
+      <c r="P124" s="20"/>
+      <c r="Q124" s="20"/>
+      <c r="R124" s="20"/>
+      <c r="S124" s="20"/>
+      <c r="T124" s="20"/>
+      <c r="U124" s="20"/>
+    </row>
+    <row r="126" spans="14:21" ht="93" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="127" spans="14:21" ht="93" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="128" spans="14:21" ht="93" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="129" spans="14:21" ht="93" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="130" spans="14:21" ht="93" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="131" spans="14:21" ht="93" customHeight="1" x14ac:dyDescent="0.3"/>
@@ -3991,26 +5248,27 @@
     <row r="133" spans="14:21" ht="93" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="134" spans="14:21" ht="93" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="135" spans="14:21" ht="93" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="136" spans="14:21" ht="93" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="137" spans="14:21" ht="93" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="138" spans="14:21" ht="93" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="144" spans="14:21" ht="15.6" x14ac:dyDescent="0.3">
-      <c r="N144" s="21"/>
-      <c r="O144" s="21"/>
-      <c r="P144" s="21"/>
-      <c r="Q144" s="21"/>
-      <c r="R144" s="21"/>
-      <c r="S144" s="21"/>
-      <c r="T144" s="21"/>
-      <c r="U144" s="21"/>
-    </row>
+    <row r="141" spans="14:21" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="N141" s="20"/>
+      <c r="O141" s="20"/>
+      <c r="P141" s="20"/>
+      <c r="Q141" s="20"/>
+      <c r="R141" s="20"/>
+      <c r="S141" s="20"/>
+      <c r="T141" s="20"/>
+      <c r="U141" s="20"/>
+    </row>
+    <row r="143" spans="14:21" ht="93" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="144" spans="14:21" ht="93" customHeight="1" x14ac:dyDescent="0.3"/>
+    <row r="145" ht="93" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="146" ht="93" customHeight="1" x14ac:dyDescent="0.3"/>
     <row r="147" ht="93" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="148" ht="93" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="149" ht="93" customHeight="1" x14ac:dyDescent="0.3"/>
-    <row r="150" ht="93" customHeight="1" x14ac:dyDescent="0.3"/>
   </sheetData>
-  <mergeCells count="26">
+  <mergeCells count="32">
+    <mergeCell ref="B61:B62"/>
+    <mergeCell ref="C61:C62"/>
+    <mergeCell ref="D61:D62"/>
+    <mergeCell ref="E61:E62"/>
     <mergeCell ref="B39:B40"/>
     <mergeCell ref="C39:C40"/>
     <mergeCell ref="D39:D40"/>
@@ -4032,6 +5290,8 @@
     <mergeCell ref="D18:D19"/>
     <mergeCell ref="E18:E19"/>
     <mergeCell ref="F18:U18"/>
+    <mergeCell ref="F61:M61"/>
+    <mergeCell ref="B60:M60"/>
     <mergeCell ref="F6:U6"/>
     <mergeCell ref="B6:B7"/>
     <mergeCell ref="C6:C7"/>

</xml_diff>